<commit_message>
updated system fact sheets to reflect db changes.
git-svn-id: svn://107.170.10.188:8080/Semoss/trunk@736 ef391c1c-ee15-45f7-b1d6-dde3d27a2169

Former-commit-id: 953ca7c775f8cb586c38651464cf387c99eb2e16
</commit_message>
<xml_diff>
--- a/export/Reports/FactSheets/Fact_Sheet_Template.xlsx
+++ b/export/Reports/FactSheets/Fact_Sheet_Template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1050" windowWidth="15120" windowHeight="6465" tabRatio="727"/>
+    <workbookView xWindow="240" yWindow="1050" windowWidth="15120" windowHeight="6465" tabRatio="727" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="System Overview" sheetId="21" r:id="rId1"/>
@@ -2331,7 +2331,6 @@
           </c:strCache>
         </c:strRef>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -2412,11 +2411,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="-25"/>
-        <c:axId val="228611584"/>
-        <c:axId val="228613120"/>
+        <c:axId val="409772800"/>
+        <c:axId val="409774336"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="228611584"/>
+        <c:axId val="409772800"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2425,7 +2424,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="228613120"/>
+        <c:crossAx val="409774336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2433,7 +2432,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="228613120"/>
+        <c:axId val="409774336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2443,7 +2442,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="228611584"/>
+        <c:crossAx val="409772800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2495,7 +2494,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2686,11 +2684,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="228267136"/>
-        <c:axId val="228268672"/>
+        <c:axId val="410036096"/>
+        <c:axId val="410037632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="228267136"/>
+        <c:axId val="410036096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2700,7 +2698,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="228268672"/>
+        <c:crossAx val="410037632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2708,7 +2706,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="228268672"/>
+        <c:axId val="410037632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2719,14 +2717,13 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="228267136"/>
+        <c:crossAx val="410036096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7018,7 +7015,7 @@
   </sheetPr>
   <dimension ref="A1:V52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="W16" sqref="W16"/>
     </sheetView>
   </sheetViews>
@@ -7662,7 +7659,7 @@
       <c r="A29" s="43"/>
       <c r="B29" s="155" t="str">
         <f ca="1">"System Hardware and Software Lifecycle support is calculated using base system hardware and software data provided by 11/30/2013 and is based upon the level of vendor hardware and software support provided as of the following date: "&amp;MONTH(TODAY())&amp;"/"&amp;DAY(TODAY())&amp;"/"&amp;YEAR(TODAY())&amp;"."</f>
-        <v>System Hardware and Software Lifecycle support is calculated using base system hardware and software data provided by 11/30/2013 and is based upon the level of vendor hardware and software support provided as of the following date: 12/9/2013.</v>
+        <v>System Hardware and Software Lifecycle support is calculated using base system hardware and software data provided by 11/30/2013 and is based upon the level of vendor hardware and software support provided as of the following date: 2/21/2014.</v>
       </c>
       <c r="C29" s="156"/>
       <c r="D29" s="156"/>
@@ -8378,10 +8375,10 @@
     <tabColor theme="4" tint="-6.1037018951994385E-5"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H263"/>
+  <dimension ref="A1:H320"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:H5"/>
+    <sheetView tabSelected="1" topLeftCell="A301" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B280" sqref="B280:H320"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10802,6 +10799,519 @@
       <c r="F263" s="36"/>
       <c r="G263" s="38"/>
       <c r="H263" s="37"/>
+    </row>
+    <row r="264" spans="2:8">
+      <c r="B264" s="39"/>
+      <c r="C264" s="36"/>
+      <c r="D264" s="37"/>
+      <c r="E264" s="37"/>
+      <c r="F264" s="36"/>
+      <c r="G264" s="38"/>
+      <c r="H264" s="37"/>
+    </row>
+    <row r="265" spans="2:8">
+      <c r="B265" s="39"/>
+      <c r="C265" s="36"/>
+      <c r="D265" s="37"/>
+      <c r="E265" s="37"/>
+      <c r="F265" s="36"/>
+      <c r="G265" s="38"/>
+      <c r="H265" s="37"/>
+    </row>
+    <row r="266" spans="2:8">
+      <c r="B266" s="39"/>
+      <c r="C266" s="36"/>
+      <c r="D266" s="37"/>
+      <c r="E266" s="37"/>
+      <c r="F266" s="36"/>
+      <c r="G266" s="38"/>
+      <c r="H266" s="37"/>
+    </row>
+    <row r="267" spans="2:8">
+      <c r="B267" s="39"/>
+      <c r="C267" s="36"/>
+      <c r="D267" s="37"/>
+      <c r="E267" s="37"/>
+      <c r="F267" s="36"/>
+      <c r="G267" s="38"/>
+      <c r="H267" s="37"/>
+    </row>
+    <row r="268" spans="2:8">
+      <c r="B268" s="39"/>
+      <c r="C268" s="36"/>
+      <c r="D268" s="37"/>
+      <c r="E268" s="37"/>
+      <c r="F268" s="36"/>
+      <c r="G268" s="38"/>
+      <c r="H268" s="37"/>
+    </row>
+    <row r="269" spans="2:8">
+      <c r="B269" s="39"/>
+      <c r="C269" s="36"/>
+      <c r="D269" s="37"/>
+      <c r="E269" s="37"/>
+      <c r="F269" s="36"/>
+      <c r="G269" s="38"/>
+      <c r="H269" s="37"/>
+    </row>
+    <row r="270" spans="2:8">
+      <c r="B270" s="39"/>
+      <c r="C270" s="36"/>
+      <c r="D270" s="37"/>
+      <c r="E270" s="37"/>
+      <c r="F270" s="36"/>
+      <c r="G270" s="38"/>
+      <c r="H270" s="37"/>
+    </row>
+    <row r="271" spans="2:8">
+      <c r="B271" s="39"/>
+      <c r="C271" s="36"/>
+      <c r="D271" s="37"/>
+      <c r="E271" s="37"/>
+      <c r="F271" s="36"/>
+      <c r="G271" s="38"/>
+      <c r="H271" s="37"/>
+    </row>
+    <row r="272" spans="2:8">
+      <c r="B272" s="39"/>
+      <c r="C272" s="36"/>
+      <c r="D272" s="37"/>
+      <c r="E272" s="37"/>
+      <c r="F272" s="36"/>
+      <c r="G272" s="38"/>
+      <c r="H272" s="37"/>
+    </row>
+    <row r="273" spans="2:8">
+      <c r="B273" s="39"/>
+      <c r="C273" s="36"/>
+      <c r="D273" s="37"/>
+      <c r="E273" s="37"/>
+      <c r="F273" s="36"/>
+      <c r="G273" s="38"/>
+      <c r="H273" s="37"/>
+    </row>
+    <row r="274" spans="2:8">
+      <c r="B274" s="39"/>
+      <c r="C274" s="36"/>
+      <c r="D274" s="37"/>
+      <c r="E274" s="37"/>
+      <c r="F274" s="36"/>
+      <c r="G274" s="38"/>
+      <c r="H274" s="37"/>
+    </row>
+    <row r="275" spans="2:8">
+      <c r="B275" s="39"/>
+      <c r="C275" s="36"/>
+      <c r="D275" s="37"/>
+      <c r="E275" s="37"/>
+      <c r="F275" s="36"/>
+      <c r="G275" s="38"/>
+      <c r="H275" s="37"/>
+    </row>
+    <row r="276" spans="2:8">
+      <c r="B276" s="39"/>
+      <c r="C276" s="36"/>
+      <c r="D276" s="37"/>
+      <c r="E276" s="37"/>
+      <c r="F276" s="36"/>
+      <c r="G276" s="38"/>
+      <c r="H276" s="37"/>
+    </row>
+    <row r="277" spans="2:8">
+      <c r="B277" s="39"/>
+      <c r="C277" s="36"/>
+      <c r="D277" s="37"/>
+      <c r="E277" s="37"/>
+      <c r="F277" s="36"/>
+      <c r="G277" s="38"/>
+      <c r="H277" s="37"/>
+    </row>
+    <row r="278" spans="2:8">
+      <c r="B278" s="39"/>
+      <c r="C278" s="36"/>
+      <c r="D278" s="37"/>
+      <c r="E278" s="37"/>
+      <c r="F278" s="36"/>
+      <c r="G278" s="38"/>
+      <c r="H278" s="37"/>
+    </row>
+    <row r="279" spans="2:8">
+      <c r="B279" s="39"/>
+      <c r="C279" s="36"/>
+      <c r="D279" s="37"/>
+      <c r="E279" s="37"/>
+      <c r="F279" s="36"/>
+      <c r="G279" s="38"/>
+      <c r="H279" s="37"/>
+    </row>
+    <row r="280" spans="2:8">
+      <c r="B280" s="39"/>
+      <c r="C280" s="36"/>
+      <c r="D280" s="37"/>
+      <c r="E280" s="37"/>
+      <c r="F280" s="36"/>
+      <c r="G280" s="38"/>
+      <c r="H280" s="37"/>
+    </row>
+    <row r="281" spans="2:8">
+      <c r="B281" s="39"/>
+      <c r="C281" s="36"/>
+      <c r="D281" s="37"/>
+      <c r="E281" s="37"/>
+      <c r="F281" s="36"/>
+      <c r="G281" s="38"/>
+      <c r="H281" s="37"/>
+    </row>
+    <row r="282" spans="2:8">
+      <c r="B282" s="39"/>
+      <c r="C282" s="36"/>
+      <c r="D282" s="37"/>
+      <c r="E282" s="37"/>
+      <c r="F282" s="36"/>
+      <c r="G282" s="38"/>
+      <c r="H282" s="37"/>
+    </row>
+    <row r="283" spans="2:8">
+      <c r="B283" s="39"/>
+      <c r="C283" s="36"/>
+      <c r="D283" s="37"/>
+      <c r="E283" s="37"/>
+      <c r="F283" s="36"/>
+      <c r="G283" s="38"/>
+      <c r="H283" s="37"/>
+    </row>
+    <row r="284" spans="2:8">
+      <c r="B284" s="39"/>
+      <c r="C284" s="36"/>
+      <c r="D284" s="37"/>
+      <c r="E284" s="37"/>
+      <c r="F284" s="36"/>
+      <c r="G284" s="38"/>
+      <c r="H284" s="37"/>
+    </row>
+    <row r="285" spans="2:8">
+      <c r="B285" s="39"/>
+      <c r="C285" s="36"/>
+      <c r="D285" s="37"/>
+      <c r="E285" s="37"/>
+      <c r="F285" s="36"/>
+      <c r="G285" s="38"/>
+      <c r="H285" s="37"/>
+    </row>
+    <row r="286" spans="2:8">
+      <c r="B286" s="39"/>
+      <c r="C286" s="36"/>
+      <c r="D286" s="37"/>
+      <c r="E286" s="37"/>
+      <c r="F286" s="36"/>
+      <c r="G286" s="38"/>
+      <c r="H286" s="37"/>
+    </row>
+    <row r="287" spans="2:8">
+      <c r="B287" s="39"/>
+      <c r="C287" s="36"/>
+      <c r="D287" s="37"/>
+      <c r="E287" s="37"/>
+      <c r="F287" s="36"/>
+      <c r="G287" s="38"/>
+      <c r="H287" s="37"/>
+    </row>
+    <row r="288" spans="2:8">
+      <c r="B288" s="39"/>
+      <c r="C288" s="36"/>
+      <c r="D288" s="37"/>
+      <c r="E288" s="37"/>
+      <c r="F288" s="36"/>
+      <c r="G288" s="38"/>
+      <c r="H288" s="37"/>
+    </row>
+    <row r="289" spans="2:8">
+      <c r="B289" s="39"/>
+      <c r="C289" s="36"/>
+      <c r="D289" s="37"/>
+      <c r="E289" s="37"/>
+      <c r="F289" s="36"/>
+      <c r="G289" s="38"/>
+      <c r="H289" s="37"/>
+    </row>
+    <row r="290" spans="2:8">
+      <c r="B290" s="39"/>
+      <c r="C290" s="36"/>
+      <c r="D290" s="37"/>
+      <c r="E290" s="37"/>
+      <c r="F290" s="36"/>
+      <c r="G290" s="38"/>
+      <c r="H290" s="37"/>
+    </row>
+    <row r="291" spans="2:8">
+      <c r="B291" s="39"/>
+      <c r="C291" s="36"/>
+      <c r="D291" s="37"/>
+      <c r="E291" s="37"/>
+      <c r="F291" s="36"/>
+      <c r="G291" s="38"/>
+      <c r="H291" s="37"/>
+    </row>
+    <row r="292" spans="2:8">
+      <c r="B292" s="39"/>
+      <c r="C292" s="36"/>
+      <c r="D292" s="37"/>
+      <c r="E292" s="37"/>
+      <c r="F292" s="36"/>
+      <c r="G292" s="38"/>
+      <c r="H292" s="37"/>
+    </row>
+    <row r="293" spans="2:8">
+      <c r="B293" s="39"/>
+      <c r="C293" s="36"/>
+      <c r="D293" s="37"/>
+      <c r="E293" s="37"/>
+      <c r="F293" s="36"/>
+      <c r="G293" s="38"/>
+      <c r="H293" s="37"/>
+    </row>
+    <row r="294" spans="2:8">
+      <c r="B294" s="39"/>
+      <c r="C294" s="36"/>
+      <c r="D294" s="37"/>
+      <c r="E294" s="37"/>
+      <c r="F294" s="36"/>
+      <c r="G294" s="38"/>
+      <c r="H294" s="37"/>
+    </row>
+    <row r="295" spans="2:8">
+      <c r="B295" s="39"/>
+      <c r="C295" s="36"/>
+      <c r="D295" s="37"/>
+      <c r="E295" s="37"/>
+      <c r="F295" s="36"/>
+      <c r="G295" s="38"/>
+      <c r="H295" s="37"/>
+    </row>
+    <row r="296" spans="2:8">
+      <c r="B296" s="39"/>
+      <c r="C296" s="36"/>
+      <c r="D296" s="37"/>
+      <c r="E296" s="37"/>
+      <c r="F296" s="36"/>
+      <c r="G296" s="38"/>
+      <c r="H296" s="37"/>
+    </row>
+    <row r="297" spans="2:8">
+      <c r="B297" s="39"/>
+      <c r="C297" s="36"/>
+      <c r="D297" s="37"/>
+      <c r="E297" s="37"/>
+      <c r="F297" s="36"/>
+      <c r="G297" s="38"/>
+      <c r="H297" s="37"/>
+    </row>
+    <row r="298" spans="2:8">
+      <c r="B298" s="39"/>
+      <c r="C298" s="36"/>
+      <c r="D298" s="37"/>
+      <c r="E298" s="37"/>
+      <c r="F298" s="36"/>
+      <c r="G298" s="38"/>
+      <c r="H298" s="37"/>
+    </row>
+    <row r="299" spans="2:8">
+      <c r="B299" s="39"/>
+      <c r="C299" s="36"/>
+      <c r="D299" s="37"/>
+      <c r="E299" s="37"/>
+      <c r="F299" s="36"/>
+      <c r="G299" s="38"/>
+      <c r="H299" s="37"/>
+    </row>
+    <row r="300" spans="2:8">
+      <c r="B300" s="39"/>
+      <c r="C300" s="36"/>
+      <c r="D300" s="37"/>
+      <c r="E300" s="37"/>
+      <c r="F300" s="36"/>
+      <c r="G300" s="38"/>
+      <c r="H300" s="37"/>
+    </row>
+    <row r="301" spans="2:8">
+      <c r="B301" s="39"/>
+      <c r="C301" s="36"/>
+      <c r="D301" s="37"/>
+      <c r="E301" s="37"/>
+      <c r="F301" s="36"/>
+      <c r="G301" s="38"/>
+      <c r="H301" s="37"/>
+    </row>
+    <row r="302" spans="2:8">
+      <c r="B302" s="39"/>
+      <c r="C302" s="36"/>
+      <c r="D302" s="37"/>
+      <c r="E302" s="37"/>
+      <c r="F302" s="36"/>
+      <c r="G302" s="38"/>
+      <c r="H302" s="37"/>
+    </row>
+    <row r="303" spans="2:8">
+      <c r="B303" s="39"/>
+      <c r="C303" s="36"/>
+      <c r="D303" s="37"/>
+      <c r="E303" s="37"/>
+      <c r="F303" s="36"/>
+      <c r="G303" s="38"/>
+      <c r="H303" s="37"/>
+    </row>
+    <row r="304" spans="2:8">
+      <c r="B304" s="39"/>
+      <c r="C304" s="36"/>
+      <c r="D304" s="37"/>
+      <c r="E304" s="37"/>
+      <c r="F304" s="36"/>
+      <c r="G304" s="38"/>
+      <c r="H304" s="37"/>
+    </row>
+    <row r="305" spans="2:8">
+      <c r="B305" s="39"/>
+      <c r="C305" s="36"/>
+      <c r="D305" s="37"/>
+      <c r="E305" s="37"/>
+      <c r="F305" s="36"/>
+      <c r="G305" s="38"/>
+      <c r="H305" s="37"/>
+    </row>
+    <row r="306" spans="2:8">
+      <c r="B306" s="39"/>
+      <c r="C306" s="36"/>
+      <c r="D306" s="37"/>
+      <c r="E306" s="37"/>
+      <c r="F306" s="36"/>
+      <c r="G306" s="38"/>
+      <c r="H306" s="37"/>
+    </row>
+    <row r="307" spans="2:8">
+      <c r="B307" s="39"/>
+      <c r="C307" s="36"/>
+      <c r="D307" s="37"/>
+      <c r="E307" s="37"/>
+      <c r="F307" s="36"/>
+      <c r="G307" s="38"/>
+      <c r="H307" s="37"/>
+    </row>
+    <row r="308" spans="2:8">
+      <c r="B308" s="39"/>
+      <c r="C308" s="36"/>
+      <c r="D308" s="37"/>
+      <c r="E308" s="37"/>
+      <c r="F308" s="36"/>
+      <c r="G308" s="38"/>
+      <c r="H308" s="37"/>
+    </row>
+    <row r="309" spans="2:8">
+      <c r="B309" s="39"/>
+      <c r="C309" s="36"/>
+      <c r="D309" s="37"/>
+      <c r="E309" s="37"/>
+      <c r="F309" s="36"/>
+      <c r="G309" s="38"/>
+      <c r="H309" s="37"/>
+    </row>
+    <row r="310" spans="2:8">
+      <c r="B310" s="39"/>
+      <c r="C310" s="36"/>
+      <c r="D310" s="37"/>
+      <c r="E310" s="37"/>
+      <c r="F310" s="36"/>
+      <c r="G310" s="38"/>
+      <c r="H310" s="37"/>
+    </row>
+    <row r="311" spans="2:8">
+      <c r="B311" s="39"/>
+      <c r="C311" s="36"/>
+      <c r="D311" s="37"/>
+      <c r="E311" s="37"/>
+      <c r="F311" s="36"/>
+      <c r="G311" s="38"/>
+      <c r="H311" s="37"/>
+    </row>
+    <row r="312" spans="2:8">
+      <c r="B312" s="39"/>
+      <c r="C312" s="36"/>
+      <c r="D312" s="37"/>
+      <c r="E312" s="37"/>
+      <c r="F312" s="36"/>
+      <c r="G312" s="38"/>
+      <c r="H312" s="37"/>
+    </row>
+    <row r="313" spans="2:8">
+      <c r="B313" s="39"/>
+      <c r="C313" s="36"/>
+      <c r="D313" s="37"/>
+      <c r="E313" s="37"/>
+      <c r="F313" s="36"/>
+      <c r="G313" s="38"/>
+      <c r="H313" s="37"/>
+    </row>
+    <row r="314" spans="2:8">
+      <c r="B314" s="39"/>
+      <c r="C314" s="36"/>
+      <c r="D314" s="37"/>
+      <c r="E314" s="37"/>
+      <c r="F314" s="36"/>
+      <c r="G314" s="38"/>
+      <c r="H314" s="37"/>
+    </row>
+    <row r="315" spans="2:8">
+      <c r="B315" s="39"/>
+      <c r="C315" s="36"/>
+      <c r="D315" s="37"/>
+      <c r="E315" s="37"/>
+      <c r="F315" s="36"/>
+      <c r="G315" s="38"/>
+      <c r="H315" s="37"/>
+    </row>
+    <row r="316" spans="2:8">
+      <c r="B316" s="39"/>
+      <c r="C316" s="36"/>
+      <c r="D316" s="37"/>
+      <c r="E316" s="37"/>
+      <c r="F316" s="36"/>
+      <c r="G316" s="38"/>
+      <c r="H316" s="37"/>
+    </row>
+    <row r="317" spans="2:8">
+      <c r="B317" s="39"/>
+      <c r="C317" s="36"/>
+      <c r="D317" s="37"/>
+      <c r="E317" s="37"/>
+      <c r="F317" s="36"/>
+      <c r="G317" s="38"/>
+      <c r="H317" s="37"/>
+    </row>
+    <row r="318" spans="2:8">
+      <c r="B318" s="39"/>
+      <c r="C318" s="36"/>
+      <c r="D318" s="37"/>
+      <c r="E318" s="37"/>
+      <c r="F318" s="36"/>
+      <c r="G318" s="38"/>
+      <c r="H318" s="37"/>
+    </row>
+    <row r="319" spans="2:8">
+      <c r="B319" s="39"/>
+      <c r="C319" s="36"/>
+      <c r="D319" s="37"/>
+      <c r="E319" s="37"/>
+      <c r="F319" s="36"/>
+      <c r="G319" s="38"/>
+      <c r="H319" s="37"/>
+    </row>
+    <row r="320" spans="2:8">
+      <c r="B320" s="39"/>
+      <c r="C320" s="36"/>
+      <c r="D320" s="37"/>
+      <c r="E320" s="37"/>
+      <c r="F320" s="36"/>
+      <c r="G320" s="38"/>
+      <c r="H320" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
updated fact sheets and image exporters
git-svn-id: svn://107.170.10.188:8080/Semoss/trunk@785 ef391c1c-ee15-45f7-b1d6-dde3d27a2169

Former-commit-id: 140626096a27853bf91860cf4a84263cd141e8a6
</commit_message>
<xml_diff>
--- a/export/Reports/FactSheets/Fact_Sheet_Template.xlsx
+++ b/export/Reports/FactSheets/Fact_Sheet_Template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1050" windowWidth="15120" windowHeight="6465" tabRatio="727" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="1050" windowWidth="15120" windowHeight="6465" tabRatio="727"/>
   </bookViews>
   <sheets>
     <sheet name="System Overview" sheetId="21" r:id="rId1"/>
@@ -1485,194 +1485,62 @@
     <xf numFmtId="9" fontId="11" fillId="0" borderId="1" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="7" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="6" xfId="50" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="7" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="7" xfId="50" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="11" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="4" xfId="50" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="12" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="5" xfId="50" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="6" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="14" fillId="0" borderId="1" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="7" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="1" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="4" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="6" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="13" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="7" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="3" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="4" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="14" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="5" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="11" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="12" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="6" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="12" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="11" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="12" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="7" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="7" borderId="11" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="7" borderId="12" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="5" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="7" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="1" xfId="50" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="6" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="7" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="4" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="5" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="7" borderId="9" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="12" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="7" borderId="4" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" xfId="50" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" xfId="50" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" xfId="50" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="5" borderId="10" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="7" borderId="5" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="5" borderId="12" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="3" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="6" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="7" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="7" borderId="12" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="11" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="12" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="20" fillId="8" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="20" fillId="8" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="20" fillId="8" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="7" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1731,59 +1599,191 @@
     <xf numFmtId="0" fontId="18" fillId="10" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="7" borderId="9" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="20" fillId="8" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="20" fillId="8" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="20" fillId="8" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="7" borderId="4" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="11" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="7" borderId="5" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="12" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="7" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="11" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="7" borderId="12" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="12" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="6" xfId="50" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="7" xfId="50" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="4" xfId="50" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="12" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="5" xfId="50" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" xfId="50" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" xfId="50" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" xfId="50" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="5" borderId="10" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="6" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="5" borderId="12" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="7" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="6" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="4" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="1" xfId="50" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="11" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="12" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="6" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="12" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="11" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="12" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="7" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="5" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="6" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="7" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="4" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="7" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="7" borderId="11" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="7" borderId="12" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="1" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="7" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="5" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="1" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="6" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="13" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="7" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="3" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="4" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="14" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="5" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1830,6 +1830,15 @@
     <xf numFmtId="0" fontId="25" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="42" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="12" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1849,15 +1858,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2411,11 +2411,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="-25"/>
-        <c:axId val="409772800"/>
-        <c:axId val="409774336"/>
+        <c:axId val="138997760"/>
+        <c:axId val="138999296"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="409772800"/>
+        <c:axId val="138997760"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2424,7 +2424,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="409774336"/>
+        <c:crossAx val="138999296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2432,7 +2432,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="409774336"/>
+        <c:axId val="138999296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2442,7 +2442,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="409772800"/>
+        <c:crossAx val="138997760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2684,11 +2684,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="410036096"/>
-        <c:axId val="410037632"/>
+        <c:axId val="139199616"/>
+        <c:axId val="139201152"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="410036096"/>
+        <c:axId val="139199616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2698,7 +2698,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="410037632"/>
+        <c:crossAx val="139201152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2706,7 +2706,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="410037632"/>
+        <c:axId val="139201152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2717,7 +2717,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="410036096"/>
+        <c:crossAx val="139199616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7015,8 +7015,8 @@
   </sheetPr>
   <dimension ref="A1:V52"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="W16" sqref="W16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="T17" sqref="T17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7026,8 +7026,8 @@
     <col min="3" max="3" width="6.7109375" style="44" customWidth="1"/>
     <col min="4" max="5" width="8" style="44" customWidth="1"/>
     <col min="6" max="6" width="8.85546875" style="44" customWidth="1"/>
-    <col min="7" max="8" width="8" style="44" customWidth="1"/>
-    <col min="9" max="9" width="7.5703125" style="44" customWidth="1"/>
+    <col min="7" max="7" width="9" style="44" customWidth="1"/>
+    <col min="8" max="9" width="7.5703125" style="44" customWidth="1"/>
     <col min="10" max="10" width="1.85546875" style="44" customWidth="1"/>
     <col min="11" max="11" width="12.42578125" style="44" customWidth="1"/>
     <col min="12" max="12" width="1.28515625" style="44" customWidth="1"/>
@@ -7039,27 +7039,27 @@
   <sheetData>
     <row r="1" spans="1:18" s="42" customFormat="1" ht="119.25" customHeight="1">
       <c r="A1" s="41"/>
-      <c r="B1" s="135" t="s">
+      <c r="B1" s="143" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="136"/>
-      <c r="D1" s="137" t="s">
+      <c r="C1" s="144"/>
+      <c r="D1" s="145" t="s">
         <v>122</v>
       </c>
-      <c r="E1" s="138"/>
-      <c r="F1" s="138"/>
-      <c r="G1" s="138"/>
-      <c r="H1" s="138"/>
-      <c r="I1" s="138"/>
-      <c r="J1" s="138"/>
-      <c r="K1" s="138"/>
-      <c r="L1" s="138"/>
-      <c r="M1" s="138"/>
-      <c r="N1" s="138"/>
-      <c r="O1" s="138"/>
-      <c r="P1" s="138"/>
-      <c r="Q1" s="138"/>
-      <c r="R1" s="139"/>
+      <c r="E1" s="146"/>
+      <c r="F1" s="146"/>
+      <c r="G1" s="146"/>
+      <c r="H1" s="146"/>
+      <c r="I1" s="146"/>
+      <c r="J1" s="146"/>
+      <c r="K1" s="146"/>
+      <c r="L1" s="146"/>
+      <c r="M1" s="146"/>
+      <c r="N1" s="146"/>
+      <c r="O1" s="146"/>
+      <c r="P1" s="146"/>
+      <c r="Q1" s="146"/>
+      <c r="R1" s="147"/>
     </row>
     <row r="2" spans="1:18" ht="5.25" customHeight="1">
       <c r="A2" s="43"/>
@@ -7083,71 +7083,71 @@
     </row>
     <row r="3" spans="1:18" ht="25.5" customHeight="1">
       <c r="A3" s="43"/>
-      <c r="B3" s="140" t="s">
+      <c r="B3" s="148" t="s">
         <v>123</v>
       </c>
-      <c r="C3" s="141"/>
-      <c r="D3" s="142"/>
-      <c r="E3" s="142"/>
-      <c r="F3" s="142"/>
-      <c r="G3" s="142"/>
-      <c r="H3" s="142"/>
-      <c r="I3" s="142"/>
-      <c r="J3" s="142"/>
-      <c r="K3" s="142"/>
-      <c r="L3" s="142"/>
-      <c r="M3" s="142"/>
-      <c r="N3" s="142"/>
-      <c r="O3" s="142"/>
-      <c r="P3" s="142"/>
-      <c r="Q3" s="142"/>
-      <c r="R3" s="142"/>
+      <c r="C3" s="149"/>
+      <c r="D3" s="150"/>
+      <c r="E3" s="150"/>
+      <c r="F3" s="150"/>
+      <c r="G3" s="150"/>
+      <c r="H3" s="150"/>
+      <c r="I3" s="150"/>
+      <c r="J3" s="150"/>
+      <c r="K3" s="150"/>
+      <c r="L3" s="150"/>
+      <c r="M3" s="150"/>
+      <c r="N3" s="150"/>
+      <c r="O3" s="150"/>
+      <c r="P3" s="150"/>
+      <c r="Q3" s="150"/>
+      <c r="R3" s="150"/>
     </row>
     <row r="4" spans="1:18" s="42" customFormat="1" ht="78.75" customHeight="1">
       <c r="A4" s="41"/>
-      <c r="B4" s="143" t="s">
+      <c r="B4" s="151" t="s">
         <v>124</v>
       </c>
-      <c r="C4" s="144"/>
-      <c r="D4" s="144"/>
-      <c r="E4" s="144"/>
-      <c r="F4" s="144"/>
-      <c r="G4" s="144"/>
-      <c r="H4" s="144"/>
-      <c r="I4" s="144"/>
-      <c r="J4" s="144"/>
-      <c r="K4" s="144"/>
-      <c r="L4" s="144"/>
-      <c r="M4" s="144"/>
-      <c r="N4" s="144"/>
-      <c r="O4" s="144"/>
-      <c r="P4" s="144"/>
-      <c r="Q4" s="144"/>
-      <c r="R4" s="145"/>
+      <c r="C4" s="152"/>
+      <c r="D4" s="152"/>
+      <c r="E4" s="152"/>
+      <c r="F4" s="152"/>
+      <c r="G4" s="152"/>
+      <c r="H4" s="152"/>
+      <c r="I4" s="152"/>
+      <c r="J4" s="152"/>
+      <c r="K4" s="152"/>
+      <c r="L4" s="152"/>
+      <c r="M4" s="152"/>
+      <c r="N4" s="152"/>
+      <c r="O4" s="152"/>
+      <c r="P4" s="152"/>
+      <c r="Q4" s="152"/>
+      <c r="R4" s="153"/>
     </row>
     <row r="5" spans="1:18" s="77" customFormat="1" ht="15" customHeight="1">
       <c r="A5" s="76"/>
-      <c r="B5" s="133" t="s">
+      <c r="B5" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="133"/>
-      <c r="D5" s="132"/>
-      <c r="E5" s="132"/>
-      <c r="F5" s="132"/>
+      <c r="C5" s="100"/>
+      <c r="D5" s="155"/>
+      <c r="E5" s="155"/>
+      <c r="F5" s="155"/>
       <c r="G5" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="131"/>
-      <c r="I5" s="131"/>
-      <c r="J5" s="131"/>
-      <c r="K5" s="131"/>
-      <c r="L5" s="133" t="s">
+      <c r="H5" s="154"/>
+      <c r="I5" s="154"/>
+      <c r="J5" s="154"/>
+      <c r="K5" s="154"/>
+      <c r="L5" s="100" t="s">
         <v>15</v>
       </c>
-      <c r="M5" s="133"/>
-      <c r="N5" s="134"/>
-      <c r="O5" s="134"/>
-      <c r="P5" s="134"/>
+      <c r="M5" s="100"/>
+      <c r="N5" s="156"/>
+      <c r="O5" s="156"/>
+      <c r="P5" s="156"/>
       <c r="Q5" s="68" t="s">
         <v>103</v>
       </c>
@@ -7177,42 +7177,42 @@
     </row>
     <row r="7" spans="1:18" s="47" customFormat="1" ht="18" customHeight="1">
       <c r="A7" s="46"/>
-      <c r="B7" s="112" t="s">
+      <c r="B7" s="157" t="s">
         <v>106</v>
       </c>
-      <c r="C7" s="113"/>
-      <c r="D7" s="113"/>
-      <c r="E7" s="113"/>
-      <c r="F7" s="113"/>
-      <c r="G7" s="113"/>
-      <c r="H7" s="113"/>
-      <c r="I7" s="114"/>
+      <c r="C7" s="158"/>
+      <c r="D7" s="158"/>
+      <c r="E7" s="158"/>
+      <c r="F7" s="158"/>
+      <c r="G7" s="158"/>
+      <c r="H7" s="158"/>
+      <c r="I7" s="159"/>
       <c r="J7" s="46"/>
-      <c r="K7" s="112" t="s">
+      <c r="K7" s="157" t="s">
         <v>39</v>
       </c>
-      <c r="L7" s="113"/>
-      <c r="M7" s="113"/>
-      <c r="N7" s="113"/>
-      <c r="O7" s="113"/>
-      <c r="P7" s="113"/>
-      <c r="Q7" s="113"/>
-      <c r="R7" s="114"/>
+      <c r="L7" s="158"/>
+      <c r="M7" s="158"/>
+      <c r="N7" s="158"/>
+      <c r="O7" s="158"/>
+      <c r="P7" s="158"/>
+      <c r="Q7" s="158"/>
+      <c r="R7" s="159"/>
     </row>
     <row r="8" spans="1:18" s="47" customFormat="1" ht="18" customHeight="1">
       <c r="A8" s="46"/>
-      <c r="B8" s="115" t="s">
+      <c r="B8" s="160" t="s">
         <v>104</v>
       </c>
-      <c r="C8" s="115"/>
-      <c r="D8" s="115" t="s">
+      <c r="C8" s="160"/>
+      <c r="D8" s="160" t="s">
         <v>105</v>
       </c>
-      <c r="E8" s="115"/>
-      <c r="F8" s="115"/>
-      <c r="G8" s="115"/>
-      <c r="H8" s="115"/>
-      <c r="I8" s="115"/>
+      <c r="E8" s="160"/>
+      <c r="F8" s="160"/>
+      <c r="G8" s="160"/>
+      <c r="H8" s="160"/>
+      <c r="I8" s="160"/>
       <c r="J8" s="46"/>
       <c r="K8" s="78"/>
       <c r="L8" s="79"/>
@@ -7225,18 +7225,18 @@
     </row>
     <row r="9" spans="1:18" ht="71.25" customHeight="1">
       <c r="A9" s="43"/>
-      <c r="B9" s="126" t="s">
+      <c r="B9" s="172" t="s">
         <v>138</v>
       </c>
-      <c r="C9" s="127"/>
-      <c r="D9" s="128" t="s">
+      <c r="C9" s="173"/>
+      <c r="D9" s="174" t="s">
         <v>136</v>
       </c>
-      <c r="E9" s="129"/>
-      <c r="F9" s="129"/>
-      <c r="G9" s="129"/>
-      <c r="H9" s="129"/>
-      <c r="I9" s="130"/>
+      <c r="E9" s="175"/>
+      <c r="F9" s="175"/>
+      <c r="G9" s="175"/>
+      <c r="H9" s="175"/>
+      <c r="I9" s="176"/>
       <c r="J9" s="43"/>
       <c r="K9" s="48"/>
       <c r="L9" s="49"/>
@@ -7249,18 +7249,18 @@
     </row>
     <row r="10" spans="1:18" ht="71.25" customHeight="1">
       <c r="A10" s="43"/>
-      <c r="B10" s="126" t="s">
+      <c r="B10" s="172" t="s">
         <v>138</v>
       </c>
-      <c r="C10" s="127"/>
-      <c r="D10" s="128" t="s">
+      <c r="C10" s="173"/>
+      <c r="D10" s="174" t="s">
         <v>135</v>
       </c>
-      <c r="E10" s="129"/>
-      <c r="F10" s="129"/>
-      <c r="G10" s="129"/>
-      <c r="H10" s="129"/>
-      <c r="I10" s="130"/>
+      <c r="E10" s="175"/>
+      <c r="F10" s="175"/>
+      <c r="G10" s="175"/>
+      <c r="H10" s="175"/>
+      <c r="I10" s="176"/>
       <c r="J10" s="43"/>
       <c r="K10" s="48"/>
       <c r="L10" s="49"/>
@@ -7273,18 +7273,18 @@
     </row>
     <row r="11" spans="1:18" ht="70.5" customHeight="1">
       <c r="A11" s="43"/>
-      <c r="B11" s="126" t="s">
+      <c r="B11" s="172" t="s">
         <v>138</v>
       </c>
-      <c r="C11" s="127"/>
-      <c r="D11" s="128" t="s">
+      <c r="C11" s="173"/>
+      <c r="D11" s="174" t="s">
         <v>137</v>
       </c>
-      <c r="E11" s="129"/>
-      <c r="F11" s="129"/>
-      <c r="G11" s="129"/>
-      <c r="H11" s="129"/>
-      <c r="I11" s="130"/>
+      <c r="E11" s="175"/>
+      <c r="F11" s="175"/>
+      <c r="G11" s="175"/>
+      <c r="H11" s="175"/>
+      <c r="I11" s="176"/>
       <c r="J11" s="43"/>
       <c r="K11" s="48"/>
       <c r="L11" s="49"/>
@@ -7321,105 +7321,105 @@
     </row>
     <row r="14" spans="1:18" s="47" customFormat="1" ht="18" customHeight="1">
       <c r="A14" s="46"/>
-      <c r="B14" s="112" t="s">
+      <c r="B14" s="157" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="113"/>
-      <c r="D14" s="113"/>
-      <c r="E14" s="113"/>
-      <c r="F14" s="113"/>
-      <c r="G14" s="113"/>
-      <c r="H14" s="113"/>
-      <c r="I14" s="113"/>
-      <c r="J14" s="113"/>
-      <c r="K14" s="113"/>
-      <c r="L14" s="113"/>
-      <c r="M14" s="113"/>
-      <c r="N14" s="113"/>
-      <c r="O14" s="113"/>
-      <c r="P14" s="113"/>
-      <c r="Q14" s="113"/>
-      <c r="R14" s="114"/>
+      <c r="C14" s="158"/>
+      <c r="D14" s="158"/>
+      <c r="E14" s="158"/>
+      <c r="F14" s="158"/>
+      <c r="G14" s="158"/>
+      <c r="H14" s="158"/>
+      <c r="I14" s="158"/>
+      <c r="J14" s="158"/>
+      <c r="K14" s="158"/>
+      <c r="L14" s="158"/>
+      <c r="M14" s="158"/>
+      <c r="N14" s="158"/>
+      <c r="O14" s="158"/>
+      <c r="P14" s="158"/>
+      <c r="Q14" s="158"/>
+      <c r="R14" s="159"/>
     </row>
     <row r="15" spans="1:18" s="47" customFormat="1" ht="14.25" customHeight="1">
       <c r="A15" s="46"/>
-      <c r="B15" s="92" t="s">
+      <c r="B15" s="167" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="92"/>
-      <c r="D15" s="92" t="s">
+      <c r="C15" s="167"/>
+      <c r="D15" s="167" t="s">
         <v>110</v>
       </c>
-      <c r="E15" s="92"/>
-      <c r="F15" s="121" t="s">
+      <c r="E15" s="167"/>
+      <c r="F15" s="166" t="s">
         <v>111</v>
       </c>
-      <c r="G15" s="121"/>
-      <c r="H15" s="122" t="s">
+      <c r="G15" s="166"/>
+      <c r="H15" s="168" t="s">
         <v>114</v>
       </c>
-      <c r="I15" s="123"/>
-      <c r="J15" s="92" t="s">
+      <c r="I15" s="169"/>
+      <c r="J15" s="167" t="s">
         <v>24</v>
       </c>
-      <c r="K15" s="92"/>
-      <c r="L15" s="92"/>
-      <c r="M15" s="92" t="s">
+      <c r="K15" s="167"/>
+      <c r="L15" s="167"/>
+      <c r="M15" s="167" t="s">
         <v>91</v>
       </c>
-      <c r="N15" s="92"/>
-      <c r="O15" s="92" t="s">
+      <c r="N15" s="167"/>
+      <c r="O15" s="167" t="s">
         <v>25</v>
       </c>
-      <c r="P15" s="92"/>
-      <c r="Q15" s="92" t="s">
+      <c r="P15" s="167"/>
+      <c r="Q15" s="167" t="s">
         <v>26</v>
       </c>
-      <c r="R15" s="92"/>
+      <c r="R15" s="167"/>
     </row>
     <row r="16" spans="1:18" ht="27.75" customHeight="1">
       <c r="A16" s="43"/>
-      <c r="B16" s="92"/>
-      <c r="C16" s="92"/>
-      <c r="D16" s="92"/>
-      <c r="E16" s="92"/>
+      <c r="B16" s="167"/>
+      <c r="C16" s="167"/>
+      <c r="D16" s="167"/>
+      <c r="E16" s="167"/>
       <c r="F16" s="54" t="s">
         <v>112</v>
       </c>
       <c r="G16" s="54" t="s">
         <v>113</v>
       </c>
-      <c r="H16" s="124"/>
-      <c r="I16" s="125"/>
-      <c r="J16" s="92"/>
-      <c r="K16" s="92"/>
-      <c r="L16" s="92"/>
-      <c r="M16" s="92"/>
-      <c r="N16" s="92"/>
-      <c r="O16" s="92"/>
-      <c r="P16" s="92"/>
-      <c r="Q16" s="92"/>
-      <c r="R16" s="92"/>
+      <c r="H16" s="170"/>
+      <c r="I16" s="171"/>
+      <c r="J16" s="167"/>
+      <c r="K16" s="167"/>
+      <c r="L16" s="167"/>
+      <c r="M16" s="167"/>
+      <c r="N16" s="167"/>
+      <c r="O16" s="167"/>
+      <c r="P16" s="167"/>
+      <c r="Q16" s="167"/>
+      <c r="R16" s="167"/>
     </row>
     <row r="17" spans="1:18" ht="42.75" customHeight="1">
       <c r="A17" s="43"/>
-      <c r="B17" s="99"/>
-      <c r="C17" s="99"/>
-      <c r="D17" s="96"/>
-      <c r="E17" s="96"/>
+      <c r="B17" s="177"/>
+      <c r="C17" s="177"/>
+      <c r="D17" s="179"/>
+      <c r="E17" s="179"/>
       <c r="F17" s="90"/>
       <c r="G17" s="89"/>
-      <c r="H17" s="97"/>
-      <c r="I17" s="98"/>
-      <c r="J17" s="99"/>
-      <c r="K17" s="99"/>
-      <c r="L17" s="99"/>
-      <c r="M17" s="100"/>
-      <c r="N17" s="100"/>
-      <c r="O17" s="96"/>
-      <c r="P17" s="96"/>
-      <c r="Q17" s="96"/>
-      <c r="R17" s="96"/>
+      <c r="H17" s="180"/>
+      <c r="I17" s="181"/>
+      <c r="J17" s="177"/>
+      <c r="K17" s="177"/>
+      <c r="L17" s="177"/>
+      <c r="M17" s="182"/>
+      <c r="N17" s="182"/>
+      <c r="O17" s="179"/>
+      <c r="P17" s="179"/>
+      <c r="Q17" s="179"/>
+      <c r="R17" s="179"/>
     </row>
     <row r="18" spans="1:18" ht="5.25" customHeight="1">
       <c r="A18" s="43"/>
@@ -7435,167 +7435,167 @@
     </row>
     <row r="19" spans="1:18" s="47" customFormat="1" ht="18" customHeight="1">
       <c r="A19" s="46"/>
-      <c r="B19" s="112" t="s">
+      <c r="B19" s="157" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="113"/>
-      <c r="D19" s="113"/>
-      <c r="E19" s="113"/>
-      <c r="F19" s="113"/>
-      <c r="G19" s="113"/>
-      <c r="H19" s="113"/>
-      <c r="I19" s="114"/>
+      <c r="C19" s="158"/>
+      <c r="D19" s="158"/>
+      <c r="E19" s="158"/>
+      <c r="F19" s="158"/>
+      <c r="G19" s="158"/>
+      <c r="H19" s="158"/>
+      <c r="I19" s="159"/>
       <c r="J19" s="46"/>
-      <c r="K19" s="146" t="s">
+      <c r="K19" s="136" t="s">
         <v>17</v>
       </c>
-      <c r="L19" s="94"/>
-      <c r="M19" s="94"/>
-      <c r="N19" s="94"/>
-      <c r="O19" s="94"/>
-      <c r="P19" s="94"/>
-      <c r="Q19" s="94"/>
-      <c r="R19" s="95"/>
+      <c r="L19" s="137"/>
+      <c r="M19" s="137"/>
+      <c r="N19" s="137"/>
+      <c r="O19" s="137"/>
+      <c r="P19" s="137"/>
+      <c r="Q19" s="137"/>
+      <c r="R19" s="138"/>
     </row>
     <row r="20" spans="1:18" ht="29.25" customHeight="1">
       <c r="A20" s="43"/>
-      <c r="B20" s="147" t="s">
+      <c r="B20" s="139" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="148"/>
-      <c r="D20" s="149"/>
-      <c r="E20" s="147" t="s">
+      <c r="C20" s="140"/>
+      <c r="D20" s="141"/>
+      <c r="E20" s="139" t="s">
         <v>33</v>
       </c>
-      <c r="F20" s="148"/>
-      <c r="G20" s="148"/>
-      <c r="H20" s="148"/>
-      <c r="I20" s="149"/>
+      <c r="F20" s="140"/>
+      <c r="G20" s="140"/>
+      <c r="H20" s="140"/>
+      <c r="I20" s="141"/>
       <c r="J20" s="43"/>
-      <c r="K20" s="150" t="s">
+      <c r="K20" s="142" t="s">
         <v>18</v>
       </c>
-      <c r="L20" s="150"/>
-      <c r="M20" s="150"/>
-      <c r="N20" s="150" t="s">
+      <c r="L20" s="142"/>
+      <c r="M20" s="142"/>
+      <c r="N20" s="142" t="s">
         <v>19</v>
       </c>
-      <c r="O20" s="150"/>
-      <c r="P20" s="150" t="s">
+      <c r="O20" s="142"/>
+      <c r="P20" s="142" t="s">
         <v>71</v>
       </c>
-      <c r="Q20" s="150"/>
-      <c r="R20" s="150"/>
+      <c r="Q20" s="142"/>
+      <c r="R20" s="142"/>
     </row>
     <row r="21" spans="1:18" ht="15.75" customHeight="1">
       <c r="A21" s="43"/>
-      <c r="B21" s="101"/>
-      <c r="C21" s="102"/>
-      <c r="D21" s="103"/>
-      <c r="E21" s="110" t="s">
+      <c r="B21" s="183"/>
+      <c r="C21" s="184"/>
+      <c r="D21" s="185"/>
+      <c r="E21" s="130" t="s">
         <v>34</v>
       </c>
-      <c r="F21" s="110"/>
-      <c r="G21" s="110"/>
-      <c r="H21" s="111"/>
-      <c r="I21" s="111"/>
+      <c r="F21" s="130"/>
+      <c r="G21" s="130"/>
+      <c r="H21" s="131"/>
+      <c r="I21" s="131"/>
       <c r="J21" s="43"/>
-      <c r="K21" s="154"/>
-      <c r="L21" s="154"/>
-      <c r="M21" s="154"/>
-      <c r="N21" s="154"/>
-      <c r="O21" s="154"/>
-      <c r="P21" s="154"/>
-      <c r="Q21" s="154"/>
-      <c r="R21" s="154"/>
+      <c r="K21" s="135"/>
+      <c r="L21" s="135"/>
+      <c r="M21" s="135"/>
+      <c r="N21" s="135"/>
+      <c r="O21" s="135"/>
+      <c r="P21" s="135"/>
+      <c r="Q21" s="135"/>
+      <c r="R21" s="135"/>
     </row>
     <row r="22" spans="1:18" ht="15.75" customHeight="1">
       <c r="A22" s="43"/>
-      <c r="B22" s="104"/>
-      <c r="C22" s="105"/>
-      <c r="D22" s="106"/>
-      <c r="E22" s="110" t="s">
+      <c r="B22" s="186"/>
+      <c r="C22" s="187"/>
+      <c r="D22" s="188"/>
+      <c r="E22" s="130" t="s">
         <v>35</v>
       </c>
-      <c r="F22" s="110"/>
-      <c r="G22" s="110"/>
-      <c r="H22" s="111"/>
-      <c r="I22" s="111"/>
+      <c r="F22" s="130"/>
+      <c r="G22" s="130"/>
+      <c r="H22" s="131"/>
+      <c r="I22" s="131"/>
       <c r="J22" s="43"/>
-      <c r="K22" s="154"/>
-      <c r="L22" s="154"/>
-      <c r="M22" s="154"/>
-      <c r="N22" s="154"/>
-      <c r="O22" s="154"/>
-      <c r="P22" s="154"/>
-      <c r="Q22" s="154"/>
-      <c r="R22" s="154"/>
+      <c r="K22" s="135"/>
+      <c r="L22" s="135"/>
+      <c r="M22" s="135"/>
+      <c r="N22" s="135"/>
+      <c r="O22" s="135"/>
+      <c r="P22" s="135"/>
+      <c r="Q22" s="135"/>
+      <c r="R22" s="135"/>
     </row>
     <row r="23" spans="1:18" ht="15.75" customHeight="1">
       <c r="A23" s="43"/>
-      <c r="B23" s="104"/>
-      <c r="C23" s="105"/>
-      <c r="D23" s="106"/>
-      <c r="E23" s="110" t="s">
+      <c r="B23" s="186"/>
+      <c r="C23" s="187"/>
+      <c r="D23" s="188"/>
+      <c r="E23" s="130" t="s">
         <v>36</v>
       </c>
-      <c r="F23" s="110"/>
-      <c r="G23" s="110"/>
-      <c r="H23" s="116"/>
-      <c r="I23" s="117"/>
+      <c r="F23" s="130"/>
+      <c r="G23" s="130"/>
+      <c r="H23" s="161"/>
+      <c r="I23" s="162"/>
       <c r="J23" s="43"/>
-      <c r="K23" s="154"/>
-      <c r="L23" s="154"/>
-      <c r="M23" s="154"/>
-      <c r="N23" s="154"/>
-      <c r="O23" s="154"/>
-      <c r="P23" s="154"/>
-      <c r="Q23" s="154"/>
-      <c r="R23" s="154"/>
+      <c r="K23" s="135"/>
+      <c r="L23" s="135"/>
+      <c r="M23" s="135"/>
+      <c r="N23" s="135"/>
+      <c r="O23" s="135"/>
+      <c r="P23" s="135"/>
+      <c r="Q23" s="135"/>
+      <c r="R23" s="135"/>
     </row>
     <row r="24" spans="1:18" ht="15.75" customHeight="1">
       <c r="A24" s="43"/>
-      <c r="B24" s="104"/>
-      <c r="C24" s="105"/>
-      <c r="D24" s="106"/>
-      <c r="E24" s="118" t="s">
+      <c r="B24" s="186"/>
+      <c r="C24" s="187"/>
+      <c r="D24" s="188"/>
+      <c r="E24" s="163" t="s">
         <v>107</v>
       </c>
-      <c r="F24" s="119"/>
-      <c r="G24" s="120"/>
-      <c r="H24" s="111"/>
-      <c r="I24" s="111"/>
+      <c r="F24" s="164"/>
+      <c r="G24" s="165"/>
+      <c r="H24" s="131"/>
+      <c r="I24" s="131"/>
       <c r="J24" s="43"/>
-      <c r="K24" s="154"/>
-      <c r="L24" s="154"/>
-      <c r="M24" s="154"/>
-      <c r="N24" s="154"/>
-      <c r="O24" s="154"/>
-      <c r="P24" s="154"/>
-      <c r="Q24" s="154"/>
-      <c r="R24" s="154"/>
+      <c r="K24" s="135"/>
+      <c r="L24" s="135"/>
+      <c r="M24" s="135"/>
+      <c r="N24" s="135"/>
+      <c r="O24" s="135"/>
+      <c r="P24" s="135"/>
+      <c r="Q24" s="135"/>
+      <c r="R24" s="135"/>
     </row>
     <row r="25" spans="1:18" ht="15.75" customHeight="1">
       <c r="A25" s="43"/>
-      <c r="B25" s="107"/>
-      <c r="C25" s="108"/>
-      <c r="D25" s="109"/>
-      <c r="E25" s="110" t="s">
+      <c r="B25" s="189"/>
+      <c r="C25" s="190"/>
+      <c r="D25" s="191"/>
+      <c r="E25" s="130" t="s">
         <v>37</v>
       </c>
-      <c r="F25" s="110"/>
-      <c r="G25" s="110"/>
-      <c r="H25" s="111"/>
-      <c r="I25" s="111"/>
+      <c r="F25" s="130"/>
+      <c r="G25" s="130"/>
+      <c r="H25" s="131"/>
+      <c r="I25" s="131"/>
       <c r="J25" s="43"/>
-      <c r="K25" s="154"/>
-      <c r="L25" s="154"/>
-      <c r="M25" s="154"/>
-      <c r="N25" s="154"/>
-      <c r="O25" s="154"/>
-      <c r="P25" s="154"/>
-      <c r="Q25" s="154"/>
-      <c r="R25" s="154"/>
+      <c r="K25" s="135"/>
+      <c r="L25" s="135"/>
+      <c r="M25" s="135"/>
+      <c r="N25" s="135"/>
+      <c r="O25" s="135"/>
+      <c r="P25" s="135"/>
+      <c r="Q25" s="135"/>
+      <c r="R25" s="135"/>
     </row>
     <row r="26" spans="1:18" ht="5.25" customHeight="1">
       <c r="A26" s="43"/>
@@ -7611,35 +7611,35 @@
     </row>
     <row r="27" spans="1:18" s="47" customFormat="1" ht="18" customHeight="1">
       <c r="A27" s="46"/>
-      <c r="B27" s="93" t="s">
+      <c r="B27" s="178" t="s">
         <v>72</v>
       </c>
-      <c r="C27" s="93"/>
-      <c r="D27" s="93"/>
-      <c r="E27" s="94" t="s">
+      <c r="C27" s="178"/>
+      <c r="D27" s="178"/>
+      <c r="E27" s="137" t="s">
         <v>68</v>
       </c>
-      <c r="F27" s="94"/>
-      <c r="G27" s="94"/>
-      <c r="H27" s="94"/>
-      <c r="I27" s="94"/>
-      <c r="J27" s="94"/>
-      <c r="K27" s="95"/>
-      <c r="L27" s="151" t="s">
+      <c r="F27" s="137"/>
+      <c r="G27" s="137"/>
+      <c r="H27" s="137"/>
+      <c r="I27" s="137"/>
+      <c r="J27" s="137"/>
+      <c r="K27" s="138"/>
+      <c r="L27" s="132" t="s">
         <v>69</v>
       </c>
-      <c r="M27" s="152"/>
-      <c r="N27" s="152"/>
-      <c r="O27" s="152"/>
-      <c r="P27" s="152"/>
-      <c r="Q27" s="152"/>
-      <c r="R27" s="153"/>
+      <c r="M27" s="133"/>
+      <c r="N27" s="133"/>
+      <c r="O27" s="133"/>
+      <c r="P27" s="133"/>
+      <c r="Q27" s="133"/>
+      <c r="R27" s="134"/>
     </row>
     <row r="28" spans="1:18" ht="141.75" customHeight="1">
       <c r="A28" s="43"/>
-      <c r="B28" s="93"/>
-      <c r="C28" s="93"/>
-      <c r="D28" s="93"/>
+      <c r="B28" s="178"/>
+      <c r="C28" s="178"/>
+      <c r="D28" s="178"/>
       <c r="E28" s="60"/>
       <c r="F28" s="60"/>
       <c r="G28" s="61"/>
@@ -7657,26 +7657,26 @@
     </row>
     <row r="29" spans="1:18" ht="27" customHeight="1">
       <c r="A29" s="43"/>
-      <c r="B29" s="155" t="str">
+      <c r="B29" s="111" t="str">
         <f ca="1">"System Hardware and Software Lifecycle support is calculated using base system hardware and software data provided by 11/30/2013 and is based upon the level of vendor hardware and software support provided as of the following date: "&amp;MONTH(TODAY())&amp;"/"&amp;DAY(TODAY())&amp;"/"&amp;YEAR(TODAY())&amp;"."</f>
-        <v>System Hardware and Software Lifecycle support is calculated using base system hardware and software data provided by 11/30/2013 and is based upon the level of vendor hardware and software support provided as of the following date: 2/21/2014.</v>
-      </c>
-      <c r="C29" s="156"/>
-      <c r="D29" s="156"/>
-      <c r="E29" s="156"/>
-      <c r="F29" s="156"/>
-      <c r="G29" s="156"/>
-      <c r="H29" s="156"/>
-      <c r="I29" s="156"/>
-      <c r="J29" s="156"/>
-      <c r="K29" s="156"/>
-      <c r="L29" s="156"/>
-      <c r="M29" s="156"/>
-      <c r="N29" s="156"/>
-      <c r="O29" s="156"/>
-      <c r="P29" s="156"/>
-      <c r="Q29" s="156"/>
-      <c r="R29" s="157"/>
+        <v>System Hardware and Software Lifecycle support is calculated using base system hardware and software data provided by 11/30/2013 and is based upon the level of vendor hardware and software support provided as of the following date: 3/13/2014.</v>
+      </c>
+      <c r="C29" s="112"/>
+      <c r="D29" s="112"/>
+      <c r="E29" s="112"/>
+      <c r="F29" s="112"/>
+      <c r="G29" s="112"/>
+      <c r="H29" s="112"/>
+      <c r="I29" s="112"/>
+      <c r="J29" s="112"/>
+      <c r="K29" s="112"/>
+      <c r="L29" s="112"/>
+      <c r="M29" s="112"/>
+      <c r="N29" s="112"/>
+      <c r="O29" s="112"/>
+      <c r="P29" s="112"/>
+      <c r="Q29" s="112"/>
+      <c r="R29" s="113"/>
     </row>
     <row r="30" spans="1:18" ht="5.25" customHeight="1">
       <c r="A30" s="43"/>
@@ -7693,103 +7693,103 @@
     </row>
     <row r="31" spans="1:18" ht="18" customHeight="1">
       <c r="A31" s="43"/>
-      <c r="B31" s="169" t="s">
+      <c r="B31" s="125" t="s">
         <v>92</v>
       </c>
-      <c r="C31" s="170"/>
-      <c r="D31" s="170"/>
-      <c r="E31" s="170"/>
-      <c r="F31" s="170"/>
-      <c r="G31" s="170"/>
-      <c r="H31" s="170"/>
-      <c r="I31" s="170"/>
-      <c r="J31" s="170"/>
-      <c r="K31" s="170"/>
-      <c r="L31" s="170"/>
-      <c r="M31" s="170"/>
-      <c r="N31" s="170"/>
-      <c r="O31" s="170"/>
-      <c r="P31" s="170"/>
-      <c r="Q31" s="170"/>
-      <c r="R31" s="171"/>
+      <c r="C31" s="126"/>
+      <c r="D31" s="126"/>
+      <c r="E31" s="126"/>
+      <c r="F31" s="126"/>
+      <c r="G31" s="126"/>
+      <c r="H31" s="126"/>
+      <c r="I31" s="126"/>
+      <c r="J31" s="126"/>
+      <c r="K31" s="126"/>
+      <c r="L31" s="126"/>
+      <c r="M31" s="126"/>
+      <c r="N31" s="126"/>
+      <c r="O31" s="126"/>
+      <c r="P31" s="126"/>
+      <c r="Q31" s="126"/>
+      <c r="R31" s="127"/>
     </row>
     <row r="32" spans="1:18" ht="27" customHeight="1">
       <c r="A32" s="43"/>
-      <c r="B32" s="158" t="s">
+      <c r="B32" s="114" t="s">
         <v>109</v>
       </c>
-      <c r="C32" s="159"/>
-      <c r="D32" s="159"/>
-      <c r="E32" s="159"/>
-      <c r="F32" s="159"/>
-      <c r="G32" s="159"/>
-      <c r="H32" s="159"/>
-      <c r="I32" s="159"/>
-      <c r="J32" s="159"/>
-      <c r="K32" s="159"/>
-      <c r="L32" s="159"/>
-      <c r="M32" s="159"/>
-      <c r="N32" s="159"/>
-      <c r="O32" s="159"/>
-      <c r="P32" s="159"/>
-      <c r="Q32" s="159"/>
-      <c r="R32" s="160"/>
+      <c r="C32" s="115"/>
+      <c r="D32" s="115"/>
+      <c r="E32" s="115"/>
+      <c r="F32" s="115"/>
+      <c r="G32" s="115"/>
+      <c r="H32" s="115"/>
+      <c r="I32" s="115"/>
+      <c r="J32" s="115"/>
+      <c r="K32" s="115"/>
+      <c r="L32" s="115"/>
+      <c r="M32" s="115"/>
+      <c r="N32" s="115"/>
+      <c r="O32" s="115"/>
+      <c r="P32" s="115"/>
+      <c r="Q32" s="115"/>
+      <c r="R32" s="116"/>
     </row>
     <row r="33" spans="1:22" ht="14.25" customHeight="1">
       <c r="A33" s="43"/>
-      <c r="B33" s="172" t="s">
+      <c r="B33" s="128" t="s">
         <v>22</v>
       </c>
-      <c r="C33" s="172"/>
-      <c r="D33" s="172"/>
-      <c r="E33" s="173" t="s">
+      <c r="C33" s="128"/>
+      <c r="D33" s="128"/>
+      <c r="E33" s="129" t="s">
         <v>53</v>
       </c>
-      <c r="F33" s="173"/>
-      <c r="G33" s="173" t="s">
+      <c r="F33" s="129"/>
+      <c r="G33" s="129" t="s">
         <v>54</v>
       </c>
-      <c r="H33" s="173"/>
-      <c r="I33" s="173" t="s">
+      <c r="H33" s="129"/>
+      <c r="I33" s="129" t="s">
         <v>55</v>
       </c>
-      <c r="J33" s="173"/>
-      <c r="K33" s="173"/>
-      <c r="L33" s="173" t="s">
+      <c r="J33" s="129"/>
+      <c r="K33" s="129"/>
+      <c r="L33" s="129" t="s">
         <v>56</v>
       </c>
-      <c r="M33" s="173"/>
-      <c r="N33" s="173" t="s">
+      <c r="M33" s="129"/>
+      <c r="N33" s="129" t="s">
         <v>57</v>
       </c>
-      <c r="O33" s="173"/>
-      <c r="P33" s="161" t="s">
+      <c r="O33" s="129"/>
+      <c r="P33" s="117" t="s">
         <v>133</v>
       </c>
-      <c r="Q33" s="162"/>
-      <c r="R33" s="163"/>
+      <c r="Q33" s="118"/>
+      <c r="R33" s="119"/>
     </row>
     <row r="34" spans="1:22" ht="42.75" customHeight="1">
       <c r="A34" s="43"/>
-      <c r="B34" s="167" t="s">
+      <c r="B34" s="123" t="s">
         <v>123</v>
       </c>
-      <c r="C34" s="167"/>
-      <c r="D34" s="167"/>
-      <c r="E34" s="168"/>
-      <c r="F34" s="168"/>
-      <c r="G34" s="168"/>
-      <c r="H34" s="168"/>
-      <c r="I34" s="168"/>
-      <c r="J34" s="168"/>
-      <c r="K34" s="168"/>
-      <c r="L34" s="168"/>
-      <c r="M34" s="168"/>
-      <c r="N34" s="168"/>
-      <c r="O34" s="168"/>
-      <c r="P34" s="164"/>
-      <c r="Q34" s="165"/>
-      <c r="R34" s="166"/>
+      <c r="C34" s="123"/>
+      <c r="D34" s="123"/>
+      <c r="E34" s="124"/>
+      <c r="F34" s="124"/>
+      <c r="G34" s="124"/>
+      <c r="H34" s="124"/>
+      <c r="I34" s="124"/>
+      <c r="J34" s="124"/>
+      <c r="K34" s="124"/>
+      <c r="L34" s="124"/>
+      <c r="M34" s="124"/>
+      <c r="N34" s="124"/>
+      <c r="O34" s="124"/>
+      <c r="P34" s="120"/>
+      <c r="Q34" s="121"/>
+      <c r="R34" s="122"/>
     </row>
     <row r="35" spans="1:22" ht="5.25" customHeight="1">
       <c r="A35" s="43"/>
@@ -7813,48 +7813,48 @@
     </row>
     <row r="36" spans="1:22" ht="16.5" customHeight="1">
       <c r="A36" s="43"/>
-      <c r="B36" s="177" t="s">
+      <c r="B36" s="108" t="s">
         <v>46</v>
       </c>
-      <c r="C36" s="177"/>
-      <c r="D36" s="177"/>
-      <c r="E36" s="177"/>
-      <c r="F36" s="177"/>
-      <c r="G36" s="177"/>
-      <c r="H36" s="177"/>
-      <c r="I36" s="177"/>
-      <c r="J36" s="177"/>
-      <c r="K36" s="177"/>
-      <c r="L36" s="177"/>
-      <c r="M36" s="177"/>
-      <c r="N36" s="177"/>
-      <c r="O36" s="177"/>
-      <c r="P36" s="177"/>
-      <c r="Q36" s="177"/>
-      <c r="R36" s="177"/>
+      <c r="C36" s="108"/>
+      <c r="D36" s="108"/>
+      <c r="E36" s="108"/>
+      <c r="F36" s="108"/>
+      <c r="G36" s="108"/>
+      <c r="H36" s="108"/>
+      <c r="I36" s="108"/>
+      <c r="J36" s="108"/>
+      <c r="K36" s="108"/>
+      <c r="L36" s="108"/>
+      <c r="M36" s="108"/>
+      <c r="N36" s="108"/>
+      <c r="O36" s="108"/>
+      <c r="P36" s="108"/>
+      <c r="Q36" s="108"/>
+      <c r="R36" s="108"/>
     </row>
     <row r="37" spans="1:22" ht="44.25" customHeight="1">
       <c r="A37" s="43"/>
-      <c r="B37" s="174" t="s">
+      <c r="B37" s="105" t="s">
         <v>129</v>
       </c>
-      <c r="C37" s="174"/>
-      <c r="D37" s="174" t="s">
+      <c r="C37" s="105"/>
+      <c r="D37" s="105" t="s">
         <v>99</v>
       </c>
-      <c r="E37" s="174"/>
-      <c r="F37" s="175" t="s">
+      <c r="E37" s="105"/>
+      <c r="F37" s="106" t="s">
         <v>130</v>
       </c>
-      <c r="G37" s="176"/>
-      <c r="H37" s="175" t="s">
+      <c r="G37" s="107"/>
+      <c r="H37" s="106" t="s">
         <v>93</v>
       </c>
-      <c r="I37" s="176"/>
-      <c r="J37" s="178" t="s">
+      <c r="I37" s="107"/>
+      <c r="J37" s="109" t="s">
         <v>98</v>
       </c>
-      <c r="K37" s="179"/>
+      <c r="K37" s="110"/>
       <c r="L37" s="43"/>
       <c r="M37" s="69"/>
       <c r="N37" s="70"/>
@@ -7873,31 +7873,31 @@
     </row>
     <row r="38" spans="1:22" ht="27" customHeight="1">
       <c r="A38" s="43"/>
-      <c r="B38" s="180">
+      <c r="B38" s="92">
         <v>0</v>
       </c>
-      <c r="C38" s="181"/>
-      <c r="D38" s="184">
+      <c r="C38" s="93"/>
+      <c r="D38" s="96">
         <v>0</v>
       </c>
-      <c r="E38" s="185"/>
-      <c r="F38" s="180">
+      <c r="E38" s="97"/>
+      <c r="F38" s="92">
         <v>0</v>
       </c>
-      <c r="G38" s="181"/>
-      <c r="H38" s="180">
+      <c r="G38" s="93"/>
+      <c r="H38" s="92">
         <v>0</v>
       </c>
-      <c r="I38" s="181"/>
-      <c r="J38" s="188">
+      <c r="I38" s="93"/>
+      <c r="J38" s="101">
         <v>0</v>
       </c>
-      <c r="K38" s="189"/>
+      <c r="K38" s="102"/>
       <c r="L38" s="71"/>
-      <c r="M38" s="133" t="s">
+      <c r="M38" s="100" t="s">
         <v>131</v>
       </c>
-      <c r="N38" s="133"/>
+      <c r="N38" s="100"/>
       <c r="O38" s="86">
         <v>0</v>
       </c>
@@ -7913,21 +7913,21 @@
     </row>
     <row r="39" spans="1:22" ht="27" customHeight="1">
       <c r="A39" s="43"/>
-      <c r="B39" s="182"/>
-      <c r="C39" s="183"/>
-      <c r="D39" s="186"/>
-      <c r="E39" s="187"/>
-      <c r="F39" s="182"/>
-      <c r="G39" s="183"/>
-      <c r="H39" s="182"/>
-      <c r="I39" s="183"/>
-      <c r="J39" s="190"/>
-      <c r="K39" s="191"/>
+      <c r="B39" s="94"/>
+      <c r="C39" s="95"/>
+      <c r="D39" s="98"/>
+      <c r="E39" s="99"/>
+      <c r="F39" s="94"/>
+      <c r="G39" s="95"/>
+      <c r="H39" s="94"/>
+      <c r="I39" s="95"/>
+      <c r="J39" s="103"/>
+      <c r="K39" s="104"/>
       <c r="L39" s="71"/>
-      <c r="M39" s="133" t="s">
+      <c r="M39" s="100" t="s">
         <v>132</v>
       </c>
-      <c r="N39" s="133"/>
+      <c r="N39" s="100"/>
       <c r="O39" s="86">
         <v>0</v>
       </c>
@@ -8207,19 +8207,66 @@
     </row>
   </sheetData>
   <mergeCells count="89">
-    <mergeCell ref="B38:C39"/>
-    <mergeCell ref="D38:E39"/>
-    <mergeCell ref="F38:G39"/>
-    <mergeCell ref="H38:I39"/>
-    <mergeCell ref="M39:N39"/>
-    <mergeCell ref="M38:N38"/>
-    <mergeCell ref="J38:K39"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="B36:R36"/>
-    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="M15:N16"/>
+    <mergeCell ref="O15:P16"/>
+    <mergeCell ref="Q15:R16"/>
+    <mergeCell ref="B27:D28"/>
+    <mergeCell ref="E27:K27"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="J17:L17"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="J15:L16"/>
+    <mergeCell ref="B21:D25"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="Q17:R17"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:I8"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="D15:E16"/>
+    <mergeCell ref="B15:C16"/>
+    <mergeCell ref="H15:I16"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:I9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:I10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:I11"/>
+    <mergeCell ref="B14:R14"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="N5:P5"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="K7:R7"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:R1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:R3"/>
+    <mergeCell ref="B4:R4"/>
+    <mergeCell ref="K19:R19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="E20:I20"/>
+    <mergeCell ref="P20:R20"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="L27:R27"/>
+    <mergeCell ref="K21:M25"/>
+    <mergeCell ref="N21:O25"/>
+    <mergeCell ref="P21:R25"/>
     <mergeCell ref="B29:R29"/>
     <mergeCell ref="B32:R32"/>
     <mergeCell ref="P33:R34"/>
@@ -8236,66 +8283,19 @@
     <mergeCell ref="I33:K33"/>
     <mergeCell ref="L33:M33"/>
     <mergeCell ref="N33:O33"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="L27:R27"/>
-    <mergeCell ref="K21:M25"/>
-    <mergeCell ref="N21:O25"/>
-    <mergeCell ref="P21:R25"/>
-    <mergeCell ref="K19:R19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="E20:I20"/>
-    <mergeCell ref="P20:R20"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="N20:O20"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:R1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:R3"/>
-    <mergeCell ref="B4:R4"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="N5:P5"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="K7:R7"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:I8"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="D15:E16"/>
-    <mergeCell ref="B15:C16"/>
-    <mergeCell ref="H15:I16"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:I9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:I10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:I11"/>
-    <mergeCell ref="B14:R14"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="M15:N16"/>
-    <mergeCell ref="O15:P16"/>
-    <mergeCell ref="Q15:R16"/>
-    <mergeCell ref="B27:D28"/>
-    <mergeCell ref="E27:K27"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="J17:L17"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="J15:L16"/>
-    <mergeCell ref="B21:D25"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="Q17:R17"/>
-    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="B36:R36"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="B38:C39"/>
+    <mergeCell ref="D38:E39"/>
+    <mergeCell ref="F38:G39"/>
+    <mergeCell ref="H38:I39"/>
+    <mergeCell ref="M39:N39"/>
+    <mergeCell ref="M38:N38"/>
+    <mergeCell ref="J38:K39"/>
   </mergeCells>
   <conditionalFormatting sqref="K28:O28 L27">
     <cfRule type="dataBar" priority="2">
@@ -8377,8 +8377,8 @@
   </sheetPr>
   <dimension ref="A1:H320"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A301" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B280" sqref="B280:H320"/>
+    <sheetView topLeftCell="A262" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F330" sqref="F330"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13916,34 +13916,34 @@
       <c r="N2" s="1"/>
     </row>
     <row r="4" spans="1:14" ht="77.25" customHeight="1">
-      <c r="B4" s="209" t="s">
+      <c r="B4" s="212" t="s">
         <v>123</v>
       </c>
-      <c r="C4" s="210"/>
-      <c r="D4" s="211" t="s">
+      <c r="C4" s="213"/>
+      <c r="D4" s="214" t="s">
         <v>117</v>
       </c>
-      <c r="E4" s="212"/>
-      <c r="F4" s="212"/>
-      <c r="G4" s="212"/>
-      <c r="H4" s="213"/>
+      <c r="E4" s="215"/>
+      <c r="F4" s="215"/>
+      <c r="G4" s="215"/>
+      <c r="H4" s="216"/>
     </row>
     <row r="6" spans="1:14" ht="21" customHeight="1">
-      <c r="B6" s="214" t="s">
+      <c r="B6" s="207" t="s">
         <v>102</v>
       </c>
-      <c r="C6" s="214"/>
-      <c r="D6" s="214"/>
-      <c r="E6" s="214"/>
-      <c r="F6" s="214"/>
-      <c r="G6" s="214"/>
-      <c r="H6" s="214"/>
+      <c r="C6" s="207"/>
+      <c r="D6" s="207"/>
+      <c r="E6" s="207"/>
+      <c r="F6" s="207"/>
+      <c r="G6" s="207"/>
+      <c r="H6" s="207"/>
     </row>
     <row r="7" spans="1:14" ht="23.25" customHeight="1">
-      <c r="B7" s="207" t="s">
+      <c r="B7" s="210" t="s">
         <v>100</v>
       </c>
-      <c r="C7" s="208"/>
+      <c r="C7" s="211"/>
       <c r="D7" s="84" t="s">
         <v>53</v>
       </c>
@@ -14043,106 +14043,106 @@
       <c r="D15"/>
     </row>
     <row r="16" spans="1:14" ht="20.25" customHeight="1">
-      <c r="B16" s="214" t="s">
+      <c r="B16" s="207" t="s">
         <v>127</v>
       </c>
-      <c r="C16" s="214"/>
-      <c r="D16" s="214"/>
-      <c r="E16" s="214"/>
-      <c r="F16" s="214"/>
-      <c r="G16" s="214"/>
-      <c r="H16" s="214"/>
+      <c r="C16" s="207"/>
+      <c r="D16" s="207"/>
+      <c r="E16" s="207"/>
+      <c r="F16" s="207"/>
+      <c r="G16" s="207"/>
+      <c r="H16" s="207"/>
     </row>
     <row r="17" spans="2:8" ht="37.5" customHeight="1">
-      <c r="B17" s="215" t="s">
+      <c r="B17" s="208" t="s">
         <v>78</v>
       </c>
-      <c r="C17" s="215"/>
-      <c r="D17" s="216" t="s">
+      <c r="C17" s="208"/>
+      <c r="D17" s="209" t="s">
         <v>125</v>
       </c>
-      <c r="E17" s="216"/>
-      <c r="F17" s="216"/>
-      <c r="G17" s="216"/>
-      <c r="H17" s="216"/>
+      <c r="E17" s="209"/>
+      <c r="F17" s="209"/>
+      <c r="G17" s="209"/>
+      <c r="H17" s="209"/>
     </row>
     <row r="18" spans="2:8" ht="37.5" customHeight="1">
-      <c r="B18" s="215" t="s">
+      <c r="B18" s="208" t="s">
         <v>79</v>
       </c>
-      <c r="C18" s="215"/>
-      <c r="D18" s="216" t="s">
+      <c r="C18" s="208"/>
+      <c r="D18" s="209" t="s">
         <v>126</v>
       </c>
-      <c r="E18" s="216"/>
-      <c r="F18" s="216"/>
-      <c r="G18" s="216"/>
-      <c r="H18" s="216"/>
+      <c r="E18" s="209"/>
+      <c r="F18" s="209"/>
+      <c r="G18" s="209"/>
+      <c r="H18" s="209"/>
     </row>
     <row r="19" spans="2:8" ht="37.5" customHeight="1">
-      <c r="B19" s="215" t="s">
+      <c r="B19" s="208" t="s">
         <v>80</v>
       </c>
-      <c r="C19" s="215"/>
-      <c r="D19" s="216" t="s">
+      <c r="C19" s="208"/>
+      <c r="D19" s="209" t="s">
         <v>85</v>
       </c>
-      <c r="E19" s="216"/>
-      <c r="F19" s="216"/>
-      <c r="G19" s="216"/>
-      <c r="H19" s="216"/>
+      <c r="E19" s="209"/>
+      <c r="F19" s="209"/>
+      <c r="G19" s="209"/>
+      <c r="H19" s="209"/>
     </row>
     <row r="20" spans="2:8" ht="37.5" customHeight="1">
-      <c r="B20" s="215" t="s">
+      <c r="B20" s="208" t="s">
         <v>81</v>
       </c>
-      <c r="C20" s="215"/>
-      <c r="D20" s="216" t="s">
+      <c r="C20" s="208"/>
+      <c r="D20" s="209" t="s">
         <v>86</v>
       </c>
-      <c r="E20" s="216"/>
-      <c r="F20" s="216"/>
-      <c r="G20" s="216"/>
-      <c r="H20" s="216"/>
+      <c r="E20" s="209"/>
+      <c r="F20" s="209"/>
+      <c r="G20" s="209"/>
+      <c r="H20" s="209"/>
     </row>
     <row r="21" spans="2:8" ht="37.5" customHeight="1">
-      <c r="B21" s="215" t="s">
+      <c r="B21" s="208" t="s">
         <v>82</v>
       </c>
-      <c r="C21" s="215"/>
-      <c r="D21" s="216" t="s">
+      <c r="C21" s="208"/>
+      <c r="D21" s="209" t="s">
         <v>87</v>
       </c>
-      <c r="E21" s="216"/>
-      <c r="F21" s="216"/>
-      <c r="G21" s="216"/>
-      <c r="H21" s="216"/>
+      <c r="E21" s="209"/>
+      <c r="F21" s="209"/>
+      <c r="G21" s="209"/>
+      <c r="H21" s="209"/>
     </row>
     <row r="22" spans="2:8" ht="37.5" customHeight="1">
-      <c r="B22" s="215" t="s">
+      <c r="B22" s="208" t="s">
         <v>83</v>
       </c>
-      <c r="C22" s="215"/>
-      <c r="D22" s="216" t="s">
+      <c r="C22" s="208"/>
+      <c r="D22" s="209" t="s">
         <v>88</v>
       </c>
-      <c r="E22" s="216"/>
-      <c r="F22" s="216"/>
-      <c r="G22" s="216"/>
-      <c r="H22" s="216"/>
+      <c r="E22" s="209"/>
+      <c r="F22" s="209"/>
+      <c r="G22" s="209"/>
+      <c r="H22" s="209"/>
     </row>
     <row r="23" spans="2:8" ht="37.5" customHeight="1">
-      <c r="B23" s="215" t="s">
+      <c r="B23" s="208" t="s">
         <v>84</v>
       </c>
-      <c r="C23" s="215"/>
-      <c r="D23" s="216" t="s">
+      <c r="C23" s="208"/>
+      <c r="D23" s="209" t="s">
         <v>89</v>
       </c>
-      <c r="E23" s="216"/>
-      <c r="F23" s="216"/>
-      <c r="G23" s="216"/>
-      <c r="H23" s="216"/>
+      <c r="E23" s="209"/>
+      <c r="F23" s="209"/>
+      <c r="G23" s="209"/>
+      <c r="H23" s="209"/>
     </row>
     <row r="24" spans="2:8" ht="15">
       <c r="B24"/>
@@ -14414,6 +14414,17 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:H4"/>
+    <mergeCell ref="B6:H6"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B16:H16"/>
     <mergeCell ref="B23:C23"/>
@@ -14430,17 +14441,6 @@
     <mergeCell ref="D21:H21"/>
     <mergeCell ref="D20:H20"/>
     <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:H4"/>
-    <mergeCell ref="B6:H6"/>
   </mergeCells>
   <conditionalFormatting sqref="D8:H14">
     <cfRule type="dataBar" priority="1">
@@ -15716,11 +15716,11 @@
         <v>123</v>
       </c>
       <c r="C4" s="228"/>
-      <c r="D4" s="211" t="s">
+      <c r="D4" s="214" t="s">
         <v>90</v>
       </c>
-      <c r="E4" s="212"/>
-      <c r="F4" s="213"/>
+      <c r="E4" s="215"/>
+      <c r="F4" s="216"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>

</xml_diff>

<commit_message>
fact sheets and system info report
git-svn-id: svn://107.170.10.188:8080/Semoss/trunk@801 ef391c1c-ee15-45f7-b1d6-dde3d27a2169
</commit_message>
<xml_diff>
--- a/export/Reports/FactSheets/Fact_Sheet_Template.xlsx
+++ b/export/Reports/FactSheets/Fact_Sheet_Template.xlsx
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="141">
   <si>
     <t>Business Logic</t>
   </si>
@@ -150,12 +150,6 @@
   </si>
   <si>
     <t>Business Processes Supported</t>
-  </si>
-  <si>
-    <t>Clinical</t>
-  </si>
-  <si>
-    <t>Logistics</t>
   </si>
   <si>
     <t>Software</t>
@@ -309,9 +303,6 @@
   </si>
   <si>
     <t>TBD</t>
-  </si>
-  <si>
-    <t>Business</t>
   </si>
   <si>
     <t>The breakdown of the system hardware and software vendor lifecycle identifies the relative number of hardware and software modules that are deployed and still receive vendor support (pre-EOL) for the base system.</t>
@@ -683,6 +674,18 @@
   </si>
   <si>
     <t>The deployment strategy maps illustrates where hardware is deployed for the base system, both within the Continental US (CONUS) and outside of the Continental US (OCONUS).</t>
+  </si>
+  <si>
+    <t>Capabilities Supported</t>
+  </si>
+  <si>
+    <t>HSD</t>
+  </si>
+  <si>
+    <t>HSS</t>
+  </si>
+  <si>
+    <t>FHP</t>
   </si>
 </sst>
 </file>
@@ -1485,62 +1488,194 @@
     <xf numFmtId="9" fontId="11" fillId="0" borderId="1" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="6" xfId="50" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="7" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="7" xfId="50" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="7" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="4" xfId="50" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="11" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="5" xfId="50" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="12" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="6" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="7" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="1" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="4" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="1" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="5" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="6" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="13" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="7" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="3" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="4" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="14" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="5" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="11" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="12" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="6" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="12" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="11" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="12" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="7" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="7" borderId="11" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="7" borderId="12" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="7" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="6" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="1" xfId="50" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="7" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="12" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" xfId="50" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" xfId="50" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" xfId="50" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="5" borderId="10" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="5" borderId="12" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="6" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="11" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="12" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="20" fillId="8" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="4" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="20" fillId="8" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="5" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="20" fillId="8" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="7" borderId="9" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="7" borderId="4" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="7" borderId="5" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="7" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="7" borderId="12" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="7" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1599,191 +1734,59 @@
     <xf numFmtId="0" fontId="18" fillId="10" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="33" fillId="7" borderId="9" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="33" fillId="7" borderId="4" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="20" fillId="8" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="7" borderId="5" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="7" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="7" borderId="12" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="6" xfId="50" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="7" xfId="50" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="4" xfId="50" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="5" xfId="50" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="6" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="7" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="4" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="5" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="6" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="20" fillId="8" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="7" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="20" fillId="8" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="4" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="5" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="11" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="12" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="11" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="12" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="12" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" xfId="50" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" xfId="50" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" xfId="50" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="5" borderId="10" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="5" borderId="12" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="3" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="6" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="1" xfId="50" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="11" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="12" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="6" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="12" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="11" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="12" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="7" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="7" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="7" borderId="11" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="7" borderId="12" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="14" fillId="0" borderId="1" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="7" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="1" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="6" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="13" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="7" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="3" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="4" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="14" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="5" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1830,15 +1833,6 @@
     <xf numFmtId="0" fontId="25" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="12" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1858,6 +1852,15 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2411,11 +2414,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="-25"/>
-        <c:axId val="138997760"/>
-        <c:axId val="138999296"/>
+        <c:axId val="181632384"/>
+        <c:axId val="181638272"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="138997760"/>
+        <c:axId val="181632384"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2424,7 +2427,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="138999296"/>
+        <c:crossAx val="181638272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2432,7 +2435,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="138999296"/>
+        <c:axId val="181638272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2442,7 +2445,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="138997760"/>
+        <c:crossAx val="181632384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2684,11 +2687,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="139199616"/>
-        <c:axId val="139201152"/>
+        <c:axId val="185983744"/>
+        <c:axId val="185985280"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="139199616"/>
+        <c:axId val="185983744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2698,7 +2701,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="139201152"/>
+        <c:crossAx val="185985280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2706,7 +2709,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="139201152"/>
+        <c:axId val="185985280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2717,7 +2720,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="139199616"/>
+        <c:crossAx val="185983744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7016,7 +7019,7 @@
   <dimension ref="A1:V52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="T17" sqref="T17"/>
+      <selection activeCell="K21" sqref="K21:M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7039,27 +7042,27 @@
   <sheetData>
     <row r="1" spans="1:18" s="42" customFormat="1" ht="119.25" customHeight="1">
       <c r="A1" s="41"/>
-      <c r="B1" s="143" t="s">
-        <v>59</v>
-      </c>
-      <c r="C1" s="144"/>
-      <c r="D1" s="145" t="s">
-        <v>122</v>
-      </c>
-      <c r="E1" s="146"/>
-      <c r="F1" s="146"/>
-      <c r="G1" s="146"/>
-      <c r="H1" s="146"/>
-      <c r="I1" s="146"/>
-      <c r="J1" s="146"/>
-      <c r="K1" s="146"/>
-      <c r="L1" s="146"/>
-      <c r="M1" s="146"/>
-      <c r="N1" s="146"/>
-      <c r="O1" s="146"/>
-      <c r="P1" s="146"/>
-      <c r="Q1" s="146"/>
-      <c r="R1" s="147"/>
+      <c r="B1" s="135" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="136"/>
+      <c r="D1" s="137" t="s">
+        <v>119</v>
+      </c>
+      <c r="E1" s="138"/>
+      <c r="F1" s="138"/>
+      <c r="G1" s="138"/>
+      <c r="H1" s="138"/>
+      <c r="I1" s="138"/>
+      <c r="J1" s="138"/>
+      <c r="K1" s="138"/>
+      <c r="L1" s="138"/>
+      <c r="M1" s="138"/>
+      <c r="N1" s="138"/>
+      <c r="O1" s="138"/>
+      <c r="P1" s="138"/>
+      <c r="Q1" s="138"/>
+      <c r="R1" s="139"/>
     </row>
     <row r="2" spans="1:18" ht="5.25" customHeight="1">
       <c r="A2" s="43"/>
@@ -7083,73 +7086,73 @@
     </row>
     <row r="3" spans="1:18" ht="25.5" customHeight="1">
       <c r="A3" s="43"/>
-      <c r="B3" s="148" t="s">
-        <v>123</v>
-      </c>
-      <c r="C3" s="149"/>
-      <c r="D3" s="150"/>
-      <c r="E3" s="150"/>
-      <c r="F3" s="150"/>
-      <c r="G3" s="150"/>
-      <c r="H3" s="150"/>
-      <c r="I3" s="150"/>
-      <c r="J3" s="150"/>
-      <c r="K3" s="150"/>
-      <c r="L3" s="150"/>
-      <c r="M3" s="150"/>
-      <c r="N3" s="150"/>
-      <c r="O3" s="150"/>
-      <c r="P3" s="150"/>
-      <c r="Q3" s="150"/>
-      <c r="R3" s="150"/>
+      <c r="B3" s="140" t="s">
+        <v>120</v>
+      </c>
+      <c r="C3" s="141"/>
+      <c r="D3" s="142"/>
+      <c r="E3" s="142"/>
+      <c r="F3" s="142"/>
+      <c r="G3" s="142"/>
+      <c r="H3" s="142"/>
+      <c r="I3" s="142"/>
+      <c r="J3" s="142"/>
+      <c r="K3" s="142"/>
+      <c r="L3" s="142"/>
+      <c r="M3" s="142"/>
+      <c r="N3" s="142"/>
+      <c r="O3" s="142"/>
+      <c r="P3" s="142"/>
+      <c r="Q3" s="142"/>
+      <c r="R3" s="142"/>
     </row>
     <row r="4" spans="1:18" s="42" customFormat="1" ht="78.75" customHeight="1">
       <c r="A4" s="41"/>
-      <c r="B4" s="151" t="s">
-        <v>124</v>
-      </c>
-      <c r="C4" s="152"/>
-      <c r="D4" s="152"/>
-      <c r="E4" s="152"/>
-      <c r="F4" s="152"/>
-      <c r="G4" s="152"/>
-      <c r="H4" s="152"/>
-      <c r="I4" s="152"/>
-      <c r="J4" s="152"/>
-      <c r="K4" s="152"/>
-      <c r="L4" s="152"/>
-      <c r="M4" s="152"/>
-      <c r="N4" s="152"/>
-      <c r="O4" s="152"/>
-      <c r="P4" s="152"/>
-      <c r="Q4" s="152"/>
-      <c r="R4" s="153"/>
+      <c r="B4" s="143" t="s">
+        <v>121</v>
+      </c>
+      <c r="C4" s="144"/>
+      <c r="D4" s="144"/>
+      <c r="E4" s="144"/>
+      <c r="F4" s="144"/>
+      <c r="G4" s="144"/>
+      <c r="H4" s="144"/>
+      <c r="I4" s="144"/>
+      <c r="J4" s="144"/>
+      <c r="K4" s="144"/>
+      <c r="L4" s="144"/>
+      <c r="M4" s="144"/>
+      <c r="N4" s="144"/>
+      <c r="O4" s="144"/>
+      <c r="P4" s="144"/>
+      <c r="Q4" s="144"/>
+      <c r="R4" s="145"/>
     </row>
     <row r="5" spans="1:18" s="77" customFormat="1" ht="15" customHeight="1">
       <c r="A5" s="76"/>
-      <c r="B5" s="100" t="s">
+      <c r="B5" s="133" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="100"/>
-      <c r="D5" s="155"/>
-      <c r="E5" s="155"/>
-      <c r="F5" s="155"/>
+      <c r="C5" s="133"/>
+      <c r="D5" s="132"/>
+      <c r="E5" s="132"/>
+      <c r="F5" s="132"/>
       <c r="G5" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="154"/>
-      <c r="I5" s="154"/>
-      <c r="J5" s="154"/>
-      <c r="K5" s="154"/>
-      <c r="L5" s="100" t="s">
+      <c r="H5" s="131"/>
+      <c r="I5" s="131"/>
+      <c r="J5" s="131"/>
+      <c r="K5" s="131"/>
+      <c r="L5" s="133" t="s">
         <v>15</v>
       </c>
-      <c r="M5" s="100"/>
-      <c r="N5" s="156"/>
-      <c r="O5" s="156"/>
-      <c r="P5" s="156"/>
+      <c r="M5" s="133"/>
+      <c r="N5" s="134"/>
+      <c r="O5" s="134"/>
+      <c r="P5" s="134"/>
       <c r="Q5" s="68" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="R5" s="83">
         <v>1</v>
@@ -7177,42 +7180,42 @@
     </row>
     <row r="7" spans="1:18" s="47" customFormat="1" ht="18" customHeight="1">
       <c r="A7" s="46"/>
-      <c r="B7" s="157" t="s">
-        <v>106</v>
-      </c>
-      <c r="C7" s="158"/>
-      <c r="D7" s="158"/>
-      <c r="E7" s="158"/>
-      <c r="F7" s="158"/>
-      <c r="G7" s="158"/>
-      <c r="H7" s="158"/>
-      <c r="I7" s="159"/>
+      <c r="B7" s="112" t="s">
+        <v>103</v>
+      </c>
+      <c r="C7" s="113"/>
+      <c r="D7" s="113"/>
+      <c r="E7" s="113"/>
+      <c r="F7" s="113"/>
+      <c r="G7" s="113"/>
+      <c r="H7" s="113"/>
+      <c r="I7" s="114"/>
       <c r="J7" s="46"/>
-      <c r="K7" s="157" t="s">
-        <v>39</v>
-      </c>
-      <c r="L7" s="158"/>
-      <c r="M7" s="158"/>
-      <c r="N7" s="158"/>
-      <c r="O7" s="158"/>
-      <c r="P7" s="158"/>
-      <c r="Q7" s="158"/>
-      <c r="R7" s="159"/>
+      <c r="K7" s="112" t="s">
+        <v>37</v>
+      </c>
+      <c r="L7" s="113"/>
+      <c r="M7" s="113"/>
+      <c r="N7" s="113"/>
+      <c r="O7" s="113"/>
+      <c r="P7" s="113"/>
+      <c r="Q7" s="113"/>
+      <c r="R7" s="114"/>
     </row>
     <row r="8" spans="1:18" s="47" customFormat="1" ht="18" customHeight="1">
       <c r="A8" s="46"/>
-      <c r="B8" s="160" t="s">
-        <v>104</v>
-      </c>
-      <c r="C8" s="160"/>
-      <c r="D8" s="160" t="s">
-        <v>105</v>
-      </c>
-      <c r="E8" s="160"/>
-      <c r="F8" s="160"/>
-      <c r="G8" s="160"/>
-      <c r="H8" s="160"/>
-      <c r="I8" s="160"/>
+      <c r="B8" s="115" t="s">
+        <v>101</v>
+      </c>
+      <c r="C8" s="115"/>
+      <c r="D8" s="115" t="s">
+        <v>102</v>
+      </c>
+      <c r="E8" s="115"/>
+      <c r="F8" s="115"/>
+      <c r="G8" s="115"/>
+      <c r="H8" s="115"/>
+      <c r="I8" s="115"/>
       <c r="J8" s="46"/>
       <c r="K8" s="78"/>
       <c r="L8" s="79"/>
@@ -7225,18 +7228,18 @@
     </row>
     <row r="9" spans="1:18" ht="71.25" customHeight="1">
       <c r="A9" s="43"/>
-      <c r="B9" s="172" t="s">
-        <v>138</v>
-      </c>
-      <c r="C9" s="173"/>
-      <c r="D9" s="174" t="s">
-        <v>136</v>
-      </c>
-      <c r="E9" s="175"/>
-      <c r="F9" s="175"/>
-      <c r="G9" s="175"/>
-      <c r="H9" s="175"/>
-      <c r="I9" s="176"/>
+      <c r="B9" s="126" t="s">
+        <v>135</v>
+      </c>
+      <c r="C9" s="127"/>
+      <c r="D9" s="128" t="s">
+        <v>133</v>
+      </c>
+      <c r="E9" s="129"/>
+      <c r="F9" s="129"/>
+      <c r="G9" s="129"/>
+      <c r="H9" s="129"/>
+      <c r="I9" s="130"/>
       <c r="J9" s="43"/>
       <c r="K9" s="48"/>
       <c r="L9" s="49"/>
@@ -7249,18 +7252,18 @@
     </row>
     <row r="10" spans="1:18" ht="71.25" customHeight="1">
       <c r="A10" s="43"/>
-      <c r="B10" s="172" t="s">
-        <v>138</v>
-      </c>
-      <c r="C10" s="173"/>
-      <c r="D10" s="174" t="s">
+      <c r="B10" s="126" t="s">
         <v>135</v>
       </c>
-      <c r="E10" s="175"/>
-      <c r="F10" s="175"/>
-      <c r="G10" s="175"/>
-      <c r="H10" s="175"/>
-      <c r="I10" s="176"/>
+      <c r="C10" s="127"/>
+      <c r="D10" s="128" t="s">
+        <v>132</v>
+      </c>
+      <c r="E10" s="129"/>
+      <c r="F10" s="129"/>
+      <c r="G10" s="129"/>
+      <c r="H10" s="129"/>
+      <c r="I10" s="130"/>
       <c r="J10" s="43"/>
       <c r="K10" s="48"/>
       <c r="L10" s="49"/>
@@ -7273,18 +7276,18 @@
     </row>
     <row r="11" spans="1:18" ht="70.5" customHeight="1">
       <c r="A11" s="43"/>
-      <c r="B11" s="172" t="s">
-        <v>138</v>
-      </c>
-      <c r="C11" s="173"/>
-      <c r="D11" s="174" t="s">
-        <v>137</v>
-      </c>
-      <c r="E11" s="175"/>
-      <c r="F11" s="175"/>
-      <c r="G11" s="175"/>
-      <c r="H11" s="175"/>
-      <c r="I11" s="176"/>
+      <c r="B11" s="126" t="s">
+        <v>135</v>
+      </c>
+      <c r="C11" s="127"/>
+      <c r="D11" s="128" t="s">
+        <v>134</v>
+      </c>
+      <c r="E11" s="129"/>
+      <c r="F11" s="129"/>
+      <c r="G11" s="129"/>
+      <c r="H11" s="129"/>
+      <c r="I11" s="130"/>
       <c r="J11" s="43"/>
       <c r="K11" s="48"/>
       <c r="L11" s="49"/>
@@ -7321,105 +7324,105 @@
     </row>
     <row r="14" spans="1:18" s="47" customFormat="1" ht="18" customHeight="1">
       <c r="A14" s="46"/>
-      <c r="B14" s="157" t="s">
+      <c r="B14" s="112" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="158"/>
-      <c r="D14" s="158"/>
-      <c r="E14" s="158"/>
-      <c r="F14" s="158"/>
-      <c r="G14" s="158"/>
-      <c r="H14" s="158"/>
-      <c r="I14" s="158"/>
-      <c r="J14" s="158"/>
-      <c r="K14" s="158"/>
-      <c r="L14" s="158"/>
-      <c r="M14" s="158"/>
-      <c r="N14" s="158"/>
-      <c r="O14" s="158"/>
-      <c r="P14" s="158"/>
-      <c r="Q14" s="158"/>
-      <c r="R14" s="159"/>
+      <c r="C14" s="113"/>
+      <c r="D14" s="113"/>
+      <c r="E14" s="113"/>
+      <c r="F14" s="113"/>
+      <c r="G14" s="113"/>
+      <c r="H14" s="113"/>
+      <c r="I14" s="113"/>
+      <c r="J14" s="113"/>
+      <c r="K14" s="113"/>
+      <c r="L14" s="113"/>
+      <c r="M14" s="113"/>
+      <c r="N14" s="113"/>
+      <c r="O14" s="113"/>
+      <c r="P14" s="113"/>
+      <c r="Q14" s="113"/>
+      <c r="R14" s="114"/>
     </row>
     <row r="15" spans="1:18" s="47" customFormat="1" ht="14.25" customHeight="1">
       <c r="A15" s="46"/>
-      <c r="B15" s="167" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" s="167"/>
-      <c r="D15" s="167" t="s">
-        <v>110</v>
-      </c>
-      <c r="E15" s="167"/>
-      <c r="F15" s="166" t="s">
+      <c r="B15" s="92" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="92"/>
+      <c r="D15" s="92" t="s">
+        <v>107</v>
+      </c>
+      <c r="E15" s="92"/>
+      <c r="F15" s="121" t="s">
+        <v>108</v>
+      </c>
+      <c r="G15" s="121"/>
+      <c r="H15" s="122" t="s">
         <v>111</v>
       </c>
-      <c r="G15" s="166"/>
-      <c r="H15" s="168" t="s">
-        <v>114</v>
-      </c>
-      <c r="I15" s="169"/>
-      <c r="J15" s="167" t="s">
+      <c r="I15" s="123"/>
+      <c r="J15" s="92" t="s">
+        <v>22</v>
+      </c>
+      <c r="K15" s="92"/>
+      <c r="L15" s="92"/>
+      <c r="M15" s="92" t="s">
+        <v>88</v>
+      </c>
+      <c r="N15" s="92"/>
+      <c r="O15" s="92" t="s">
+        <v>23</v>
+      </c>
+      <c r="P15" s="92"/>
+      <c r="Q15" s="92" t="s">
         <v>24</v>
       </c>
-      <c r="K15" s="167"/>
-      <c r="L15" s="167"/>
-      <c r="M15" s="167" t="s">
-        <v>91</v>
-      </c>
-      <c r="N15" s="167"/>
-      <c r="O15" s="167" t="s">
-        <v>25</v>
-      </c>
-      <c r="P15" s="167"/>
-      <c r="Q15" s="167" t="s">
-        <v>26</v>
-      </c>
-      <c r="R15" s="167"/>
+      <c r="R15" s="92"/>
     </row>
     <row r="16" spans="1:18" ht="27.75" customHeight="1">
       <c r="A16" s="43"/>
-      <c r="B16" s="167"/>
-      <c r="C16" s="167"/>
-      <c r="D16" s="167"/>
-      <c r="E16" s="167"/>
+      <c r="B16" s="92"/>
+      <c r="C16" s="92"/>
+      <c r="D16" s="92"/>
+      <c r="E16" s="92"/>
       <c r="F16" s="54" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G16" s="54" t="s">
-        <v>113</v>
-      </c>
-      <c r="H16" s="170"/>
-      <c r="I16" s="171"/>
-      <c r="J16" s="167"/>
-      <c r="K16" s="167"/>
-      <c r="L16" s="167"/>
-      <c r="M16" s="167"/>
-      <c r="N16" s="167"/>
-      <c r="O16" s="167"/>
-      <c r="P16" s="167"/>
-      <c r="Q16" s="167"/>
-      <c r="R16" s="167"/>
+        <v>110</v>
+      </c>
+      <c r="H16" s="124"/>
+      <c r="I16" s="125"/>
+      <c r="J16" s="92"/>
+      <c r="K16" s="92"/>
+      <c r="L16" s="92"/>
+      <c r="M16" s="92"/>
+      <c r="N16" s="92"/>
+      <c r="O16" s="92"/>
+      <c r="P16" s="92"/>
+      <c r="Q16" s="92"/>
+      <c r="R16" s="92"/>
     </row>
     <row r="17" spans="1:18" ht="42.75" customHeight="1">
       <c r="A17" s="43"/>
-      <c r="B17" s="177"/>
-      <c r="C17" s="177"/>
-      <c r="D17" s="179"/>
-      <c r="E17" s="179"/>
+      <c r="B17" s="99"/>
+      <c r="C17" s="99"/>
+      <c r="D17" s="96"/>
+      <c r="E17" s="96"/>
       <c r="F17" s="90"/>
       <c r="G17" s="89"/>
-      <c r="H17" s="180"/>
-      <c r="I17" s="181"/>
-      <c r="J17" s="177"/>
-      <c r="K17" s="177"/>
-      <c r="L17" s="177"/>
-      <c r="M17" s="182"/>
-      <c r="N17" s="182"/>
-      <c r="O17" s="179"/>
-      <c r="P17" s="179"/>
-      <c r="Q17" s="179"/>
-      <c r="R17" s="179"/>
+      <c r="H17" s="97"/>
+      <c r="I17" s="98"/>
+      <c r="J17" s="99"/>
+      <c r="K17" s="99"/>
+      <c r="L17" s="99"/>
+      <c r="M17" s="100"/>
+      <c r="N17" s="100"/>
+      <c r="O17" s="96"/>
+      <c r="P17" s="96"/>
+      <c r="Q17" s="96"/>
+      <c r="R17" s="96"/>
     </row>
     <row r="18" spans="1:18" ht="5.25" customHeight="1">
       <c r="A18" s="43"/>
@@ -7435,167 +7438,167 @@
     </row>
     <row r="19" spans="1:18" s="47" customFormat="1" ht="18" customHeight="1">
       <c r="A19" s="46"/>
-      <c r="B19" s="157" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="158"/>
-      <c r="D19" s="158"/>
-      <c r="E19" s="158"/>
-      <c r="F19" s="158"/>
-      <c r="G19" s="158"/>
-      <c r="H19" s="158"/>
-      <c r="I19" s="159"/>
+      <c r="B19" s="112" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="113"/>
+      <c r="D19" s="113"/>
+      <c r="E19" s="113"/>
+      <c r="F19" s="113"/>
+      <c r="G19" s="113"/>
+      <c r="H19" s="113"/>
+      <c r="I19" s="114"/>
       <c r="J19" s="46"/>
-      <c r="K19" s="136" t="s">
-        <v>17</v>
-      </c>
-      <c r="L19" s="137"/>
-      <c r="M19" s="137"/>
-      <c r="N19" s="137"/>
-      <c r="O19" s="137"/>
-      <c r="P19" s="137"/>
-      <c r="Q19" s="137"/>
-      <c r="R19" s="138"/>
+      <c r="K19" s="146" t="s">
+        <v>137</v>
+      </c>
+      <c r="L19" s="94"/>
+      <c r="M19" s="94"/>
+      <c r="N19" s="94"/>
+      <c r="O19" s="94"/>
+      <c r="P19" s="94"/>
+      <c r="Q19" s="94"/>
+      <c r="R19" s="95"/>
     </row>
     <row r="20" spans="1:18" ht="29.25" customHeight="1">
       <c r="A20" s="43"/>
-      <c r="B20" s="139" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="140"/>
-      <c r="D20" s="141"/>
-      <c r="E20" s="139" t="s">
-        <v>33</v>
-      </c>
-      <c r="F20" s="140"/>
-      <c r="G20" s="140"/>
-      <c r="H20" s="140"/>
-      <c r="I20" s="141"/>
+      <c r="B20" s="147" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="148"/>
+      <c r="D20" s="149"/>
+      <c r="E20" s="147" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20" s="148"/>
+      <c r="G20" s="148"/>
+      <c r="H20" s="148"/>
+      <c r="I20" s="149"/>
       <c r="J20" s="43"/>
-      <c r="K20" s="142" t="s">
-        <v>18</v>
-      </c>
-      <c r="L20" s="142"/>
-      <c r="M20" s="142"/>
-      <c r="N20" s="142" t="s">
-        <v>19</v>
-      </c>
-      <c r="O20" s="142"/>
-      <c r="P20" s="142" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q20" s="142"/>
-      <c r="R20" s="142"/>
+      <c r="K20" s="150" t="s">
+        <v>138</v>
+      </c>
+      <c r="L20" s="150"/>
+      <c r="M20" s="150"/>
+      <c r="N20" s="150" t="s">
+        <v>139</v>
+      </c>
+      <c r="O20" s="150"/>
+      <c r="P20" s="150" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q20" s="150"/>
+      <c r="R20" s="150"/>
     </row>
     <row r="21" spans="1:18" ht="15.75" customHeight="1">
       <c r="A21" s="43"/>
-      <c r="B21" s="183"/>
-      <c r="C21" s="184"/>
-      <c r="D21" s="185"/>
-      <c r="E21" s="130" t="s">
-        <v>34</v>
-      </c>
-      <c r="F21" s="130"/>
-      <c r="G21" s="130"/>
-      <c r="H21" s="131"/>
-      <c r="I21" s="131"/>
+      <c r="B21" s="101"/>
+      <c r="C21" s="102"/>
+      <c r="D21" s="103"/>
+      <c r="E21" s="110" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21" s="110"/>
+      <c r="G21" s="110"/>
+      <c r="H21" s="111"/>
+      <c r="I21" s="111"/>
       <c r="J21" s="43"/>
-      <c r="K21" s="135"/>
-      <c r="L21" s="135"/>
-      <c r="M21" s="135"/>
-      <c r="N21" s="135"/>
-      <c r="O21" s="135"/>
-      <c r="P21" s="135"/>
-      <c r="Q21" s="135"/>
-      <c r="R21" s="135"/>
+      <c r="K21" s="154"/>
+      <c r="L21" s="154"/>
+      <c r="M21" s="154"/>
+      <c r="N21" s="154"/>
+      <c r="O21" s="154"/>
+      <c r="P21" s="154"/>
+      <c r="Q21" s="154"/>
+      <c r="R21" s="154"/>
     </row>
     <row r="22" spans="1:18" ht="15.75" customHeight="1">
       <c r="A22" s="43"/>
-      <c r="B22" s="186"/>
-      <c r="C22" s="187"/>
-      <c r="D22" s="188"/>
-      <c r="E22" s="130" t="s">
-        <v>35</v>
-      </c>
-      <c r="F22" s="130"/>
-      <c r="G22" s="130"/>
-      <c r="H22" s="131"/>
-      <c r="I22" s="131"/>
+      <c r="B22" s="104"/>
+      <c r="C22" s="105"/>
+      <c r="D22" s="106"/>
+      <c r="E22" s="110" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" s="110"/>
+      <c r="G22" s="110"/>
+      <c r="H22" s="111"/>
+      <c r="I22" s="111"/>
       <c r="J22" s="43"/>
-      <c r="K22" s="135"/>
-      <c r="L22" s="135"/>
-      <c r="M22" s="135"/>
-      <c r="N22" s="135"/>
-      <c r="O22" s="135"/>
-      <c r="P22" s="135"/>
-      <c r="Q22" s="135"/>
-      <c r="R22" s="135"/>
+      <c r="K22" s="154"/>
+      <c r="L22" s="154"/>
+      <c r="M22" s="154"/>
+      <c r="N22" s="154"/>
+      <c r="O22" s="154"/>
+      <c r="P22" s="154"/>
+      <c r="Q22" s="154"/>
+      <c r="R22" s="154"/>
     </row>
     <row r="23" spans="1:18" ht="15.75" customHeight="1">
       <c r="A23" s="43"/>
-      <c r="B23" s="186"/>
-      <c r="C23" s="187"/>
-      <c r="D23" s="188"/>
-      <c r="E23" s="130" t="s">
-        <v>36</v>
-      </c>
-      <c r="F23" s="130"/>
-      <c r="G23" s="130"/>
-      <c r="H23" s="161"/>
-      <c r="I23" s="162"/>
+      <c r="B23" s="104"/>
+      <c r="C23" s="105"/>
+      <c r="D23" s="106"/>
+      <c r="E23" s="110" t="s">
+        <v>34</v>
+      </c>
+      <c r="F23" s="110"/>
+      <c r="G23" s="110"/>
+      <c r="H23" s="116"/>
+      <c r="I23" s="117"/>
       <c r="J23" s="43"/>
-      <c r="K23" s="135"/>
-      <c r="L23" s="135"/>
-      <c r="M23" s="135"/>
-      <c r="N23" s="135"/>
-      <c r="O23" s="135"/>
-      <c r="P23" s="135"/>
-      <c r="Q23" s="135"/>
-      <c r="R23" s="135"/>
+      <c r="K23" s="154"/>
+      <c r="L23" s="154"/>
+      <c r="M23" s="154"/>
+      <c r="N23" s="154"/>
+      <c r="O23" s="154"/>
+      <c r="P23" s="154"/>
+      <c r="Q23" s="154"/>
+      <c r="R23" s="154"/>
     </row>
     <row r="24" spans="1:18" ht="15.75" customHeight="1">
       <c r="A24" s="43"/>
-      <c r="B24" s="186"/>
-      <c r="C24" s="187"/>
-      <c r="D24" s="188"/>
-      <c r="E24" s="163" t="s">
-        <v>107</v>
-      </c>
-      <c r="F24" s="164"/>
-      <c r="G24" s="165"/>
-      <c r="H24" s="131"/>
-      <c r="I24" s="131"/>
+      <c r="B24" s="104"/>
+      <c r="C24" s="105"/>
+      <c r="D24" s="106"/>
+      <c r="E24" s="118" t="s">
+        <v>104</v>
+      </c>
+      <c r="F24" s="119"/>
+      <c r="G24" s="120"/>
+      <c r="H24" s="111"/>
+      <c r="I24" s="111"/>
       <c r="J24" s="43"/>
-      <c r="K24" s="135"/>
-      <c r="L24" s="135"/>
-      <c r="M24" s="135"/>
-      <c r="N24" s="135"/>
-      <c r="O24" s="135"/>
-      <c r="P24" s="135"/>
-      <c r="Q24" s="135"/>
-      <c r="R24" s="135"/>
+      <c r="K24" s="154"/>
+      <c r="L24" s="154"/>
+      <c r="M24" s="154"/>
+      <c r="N24" s="154"/>
+      <c r="O24" s="154"/>
+      <c r="P24" s="154"/>
+      <c r="Q24" s="154"/>
+      <c r="R24" s="154"/>
     </row>
     <row r="25" spans="1:18" ht="15.75" customHeight="1">
       <c r="A25" s="43"/>
-      <c r="B25" s="189"/>
-      <c r="C25" s="190"/>
-      <c r="D25" s="191"/>
-      <c r="E25" s="130" t="s">
-        <v>37</v>
-      </c>
-      <c r="F25" s="130"/>
-      <c r="G25" s="130"/>
-      <c r="H25" s="131"/>
-      <c r="I25" s="131"/>
+      <c r="B25" s="107"/>
+      <c r="C25" s="108"/>
+      <c r="D25" s="109"/>
+      <c r="E25" s="110" t="s">
+        <v>35</v>
+      </c>
+      <c r="F25" s="110"/>
+      <c r="G25" s="110"/>
+      <c r="H25" s="111"/>
+      <c r="I25" s="111"/>
       <c r="J25" s="43"/>
-      <c r="K25" s="135"/>
-      <c r="L25" s="135"/>
-      <c r="M25" s="135"/>
-      <c r="N25" s="135"/>
-      <c r="O25" s="135"/>
-      <c r="P25" s="135"/>
-      <c r="Q25" s="135"/>
-      <c r="R25" s="135"/>
+      <c r="K25" s="154"/>
+      <c r="L25" s="154"/>
+      <c r="M25" s="154"/>
+      <c r="N25" s="154"/>
+      <c r="O25" s="154"/>
+      <c r="P25" s="154"/>
+      <c r="Q25" s="154"/>
+      <c r="R25" s="154"/>
     </row>
     <row r="26" spans="1:18" ht="5.25" customHeight="1">
       <c r="A26" s="43"/>
@@ -7611,35 +7614,35 @@
     </row>
     <row r="27" spans="1:18" s="47" customFormat="1" ht="18" customHeight="1">
       <c r="A27" s="46"/>
-      <c r="B27" s="178" t="s">
-        <v>72</v>
-      </c>
-      <c r="C27" s="178"/>
-      <c r="D27" s="178"/>
-      <c r="E27" s="137" t="s">
-        <v>68</v>
-      </c>
-      <c r="F27" s="137"/>
-      <c r="G27" s="137"/>
-      <c r="H27" s="137"/>
-      <c r="I27" s="137"/>
-      <c r="J27" s="137"/>
-      <c r="K27" s="138"/>
-      <c r="L27" s="132" t="s">
+      <c r="B27" s="93" t="s">
         <v>69</v>
       </c>
-      <c r="M27" s="133"/>
-      <c r="N27" s="133"/>
-      <c r="O27" s="133"/>
-      <c r="P27" s="133"/>
-      <c r="Q27" s="133"/>
-      <c r="R27" s="134"/>
+      <c r="C27" s="93"/>
+      <c r="D27" s="93"/>
+      <c r="E27" s="94" t="s">
+        <v>66</v>
+      </c>
+      <c r="F27" s="94"/>
+      <c r="G27" s="94"/>
+      <c r="H27" s="94"/>
+      <c r="I27" s="94"/>
+      <c r="J27" s="94"/>
+      <c r="K27" s="95"/>
+      <c r="L27" s="151" t="s">
+        <v>67</v>
+      </c>
+      <c r="M27" s="152"/>
+      <c r="N27" s="152"/>
+      <c r="O27" s="152"/>
+      <c r="P27" s="152"/>
+      <c r="Q27" s="152"/>
+      <c r="R27" s="153"/>
     </row>
     <row r="28" spans="1:18" ht="141.75" customHeight="1">
       <c r="A28" s="43"/>
-      <c r="B28" s="178"/>
-      <c r="C28" s="178"/>
-      <c r="D28" s="178"/>
+      <c r="B28" s="93"/>
+      <c r="C28" s="93"/>
+      <c r="D28" s="93"/>
       <c r="E28" s="60"/>
       <c r="F28" s="60"/>
       <c r="G28" s="61"/>
@@ -7657,26 +7660,26 @@
     </row>
     <row r="29" spans="1:18" ht="27" customHeight="1">
       <c r="A29" s="43"/>
-      <c r="B29" s="111" t="str">
+      <c r="B29" s="155" t="str">
         <f ca="1">"System Hardware and Software Lifecycle support is calculated using base system hardware and software data provided by 11/30/2013 and is based upon the level of vendor hardware and software support provided as of the following date: "&amp;MONTH(TODAY())&amp;"/"&amp;DAY(TODAY())&amp;"/"&amp;YEAR(TODAY())&amp;"."</f>
         <v>System Hardware and Software Lifecycle support is calculated using base system hardware and software data provided by 11/30/2013 and is based upon the level of vendor hardware and software support provided as of the following date: 3/13/2014.</v>
       </c>
-      <c r="C29" s="112"/>
-      <c r="D29" s="112"/>
-      <c r="E29" s="112"/>
-      <c r="F29" s="112"/>
-      <c r="G29" s="112"/>
-      <c r="H29" s="112"/>
-      <c r="I29" s="112"/>
-      <c r="J29" s="112"/>
-      <c r="K29" s="112"/>
-      <c r="L29" s="112"/>
-      <c r="M29" s="112"/>
-      <c r="N29" s="112"/>
-      <c r="O29" s="112"/>
-      <c r="P29" s="112"/>
-      <c r="Q29" s="112"/>
-      <c r="R29" s="113"/>
+      <c r="C29" s="156"/>
+      <c r="D29" s="156"/>
+      <c r="E29" s="156"/>
+      <c r="F29" s="156"/>
+      <c r="G29" s="156"/>
+      <c r="H29" s="156"/>
+      <c r="I29" s="156"/>
+      <c r="J29" s="156"/>
+      <c r="K29" s="156"/>
+      <c r="L29" s="156"/>
+      <c r="M29" s="156"/>
+      <c r="N29" s="156"/>
+      <c r="O29" s="156"/>
+      <c r="P29" s="156"/>
+      <c r="Q29" s="156"/>
+      <c r="R29" s="157"/>
     </row>
     <row r="30" spans="1:18" ht="5.25" customHeight="1">
       <c r="A30" s="43"/>
@@ -7693,103 +7696,103 @@
     </row>
     <row r="31" spans="1:18" ht="18" customHeight="1">
       <c r="A31" s="43"/>
-      <c r="B31" s="125" t="s">
-        <v>92</v>
-      </c>
-      <c r="C31" s="126"/>
-      <c r="D31" s="126"/>
-      <c r="E31" s="126"/>
-      <c r="F31" s="126"/>
-      <c r="G31" s="126"/>
-      <c r="H31" s="126"/>
-      <c r="I31" s="126"/>
-      <c r="J31" s="126"/>
-      <c r="K31" s="126"/>
-      <c r="L31" s="126"/>
-      <c r="M31" s="126"/>
-      <c r="N31" s="126"/>
-      <c r="O31" s="126"/>
-      <c r="P31" s="126"/>
-      <c r="Q31" s="126"/>
-      <c r="R31" s="127"/>
+      <c r="B31" s="169" t="s">
+        <v>89</v>
+      </c>
+      <c r="C31" s="170"/>
+      <c r="D31" s="170"/>
+      <c r="E31" s="170"/>
+      <c r="F31" s="170"/>
+      <c r="G31" s="170"/>
+      <c r="H31" s="170"/>
+      <c r="I31" s="170"/>
+      <c r="J31" s="170"/>
+      <c r="K31" s="170"/>
+      <c r="L31" s="170"/>
+      <c r="M31" s="170"/>
+      <c r="N31" s="170"/>
+      <c r="O31" s="170"/>
+      <c r="P31" s="170"/>
+      <c r="Q31" s="170"/>
+      <c r="R31" s="171"/>
     </row>
     <row r="32" spans="1:18" ht="27" customHeight="1">
       <c r="A32" s="43"/>
-      <c r="B32" s="114" t="s">
-        <v>109</v>
-      </c>
-      <c r="C32" s="115"/>
-      <c r="D32" s="115"/>
-      <c r="E32" s="115"/>
-      <c r="F32" s="115"/>
-      <c r="G32" s="115"/>
-      <c r="H32" s="115"/>
-      <c r="I32" s="115"/>
-      <c r="J32" s="115"/>
-      <c r="K32" s="115"/>
-      <c r="L32" s="115"/>
-      <c r="M32" s="115"/>
-      <c r="N32" s="115"/>
-      <c r="O32" s="115"/>
-      <c r="P32" s="115"/>
-      <c r="Q32" s="115"/>
-      <c r="R32" s="116"/>
+      <c r="B32" s="158" t="s">
+        <v>106</v>
+      </c>
+      <c r="C32" s="159"/>
+      <c r="D32" s="159"/>
+      <c r="E32" s="159"/>
+      <c r="F32" s="159"/>
+      <c r="G32" s="159"/>
+      <c r="H32" s="159"/>
+      <c r="I32" s="159"/>
+      <c r="J32" s="159"/>
+      <c r="K32" s="159"/>
+      <c r="L32" s="159"/>
+      <c r="M32" s="159"/>
+      <c r="N32" s="159"/>
+      <c r="O32" s="159"/>
+      <c r="P32" s="159"/>
+      <c r="Q32" s="159"/>
+      <c r="R32" s="160"/>
     </row>
     <row r="33" spans="1:22" ht="14.25" customHeight="1">
       <c r="A33" s="43"/>
-      <c r="B33" s="128" t="s">
-        <v>22</v>
-      </c>
-      <c r="C33" s="128"/>
-      <c r="D33" s="128"/>
-      <c r="E33" s="129" t="s">
+      <c r="B33" s="172" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" s="172"/>
+      <c r="D33" s="172"/>
+      <c r="E33" s="173" t="s">
+        <v>51</v>
+      </c>
+      <c r="F33" s="173"/>
+      <c r="G33" s="173" t="s">
+        <v>52</v>
+      </c>
+      <c r="H33" s="173"/>
+      <c r="I33" s="173" t="s">
         <v>53</v>
       </c>
-      <c r="F33" s="129"/>
-      <c r="G33" s="129" t="s">
+      <c r="J33" s="173"/>
+      <c r="K33" s="173"/>
+      <c r="L33" s="173" t="s">
         <v>54</v>
       </c>
-      <c r="H33" s="129"/>
-      <c r="I33" s="129" t="s">
+      <c r="M33" s="173"/>
+      <c r="N33" s="173" t="s">
         <v>55</v>
       </c>
-      <c r="J33" s="129"/>
-      <c r="K33" s="129"/>
-      <c r="L33" s="129" t="s">
-        <v>56</v>
-      </c>
-      <c r="M33" s="129"/>
-      <c r="N33" s="129" t="s">
-        <v>57</v>
-      </c>
-      <c r="O33" s="129"/>
-      <c r="P33" s="117" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q33" s="118"/>
-      <c r="R33" s="119"/>
+      <c r="O33" s="173"/>
+      <c r="P33" s="161" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q33" s="162"/>
+      <c r="R33" s="163"/>
     </row>
     <row r="34" spans="1:22" ht="42.75" customHeight="1">
       <c r="A34" s="43"/>
-      <c r="B34" s="123" t="s">
-        <v>123</v>
-      </c>
-      <c r="C34" s="123"/>
-      <c r="D34" s="123"/>
-      <c r="E34" s="124"/>
-      <c r="F34" s="124"/>
-      <c r="G34" s="124"/>
-      <c r="H34" s="124"/>
-      <c r="I34" s="124"/>
-      <c r="J34" s="124"/>
-      <c r="K34" s="124"/>
-      <c r="L34" s="124"/>
-      <c r="M34" s="124"/>
-      <c r="N34" s="124"/>
-      <c r="O34" s="124"/>
-      <c r="P34" s="120"/>
-      <c r="Q34" s="121"/>
-      <c r="R34" s="122"/>
+      <c r="B34" s="167" t="s">
+        <v>120</v>
+      </c>
+      <c r="C34" s="167"/>
+      <c r="D34" s="167"/>
+      <c r="E34" s="168"/>
+      <c r="F34" s="168"/>
+      <c r="G34" s="168"/>
+      <c r="H34" s="168"/>
+      <c r="I34" s="168"/>
+      <c r="J34" s="168"/>
+      <c r="K34" s="168"/>
+      <c r="L34" s="168"/>
+      <c r="M34" s="168"/>
+      <c r="N34" s="168"/>
+      <c r="O34" s="168"/>
+      <c r="P34" s="164"/>
+      <c r="Q34" s="165"/>
+      <c r="R34" s="166"/>
     </row>
     <row r="35" spans="1:22" ht="5.25" customHeight="1">
       <c r="A35" s="43"/>
@@ -7813,48 +7816,48 @@
     </row>
     <row r="36" spans="1:22" ht="16.5" customHeight="1">
       <c r="A36" s="43"/>
-      <c r="B36" s="108" t="s">
-        <v>46</v>
-      </c>
-      <c r="C36" s="108"/>
-      <c r="D36" s="108"/>
-      <c r="E36" s="108"/>
-      <c r="F36" s="108"/>
-      <c r="G36" s="108"/>
-      <c r="H36" s="108"/>
-      <c r="I36" s="108"/>
-      <c r="J36" s="108"/>
-      <c r="K36" s="108"/>
-      <c r="L36" s="108"/>
-      <c r="M36" s="108"/>
-      <c r="N36" s="108"/>
-      <c r="O36" s="108"/>
-      <c r="P36" s="108"/>
-      <c r="Q36" s="108"/>
-      <c r="R36" s="108"/>
+      <c r="B36" s="177" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36" s="177"/>
+      <c r="D36" s="177"/>
+      <c r="E36" s="177"/>
+      <c r="F36" s="177"/>
+      <c r="G36" s="177"/>
+      <c r="H36" s="177"/>
+      <c r="I36" s="177"/>
+      <c r="J36" s="177"/>
+      <c r="K36" s="177"/>
+      <c r="L36" s="177"/>
+      <c r="M36" s="177"/>
+      <c r="N36" s="177"/>
+      <c r="O36" s="177"/>
+      <c r="P36" s="177"/>
+      <c r="Q36" s="177"/>
+      <c r="R36" s="177"/>
     </row>
     <row r="37" spans="1:22" ht="44.25" customHeight="1">
       <c r="A37" s="43"/>
-      <c r="B37" s="105" t="s">
-        <v>129</v>
-      </c>
-      <c r="C37" s="105"/>
-      <c r="D37" s="105" t="s">
-        <v>99</v>
-      </c>
-      <c r="E37" s="105"/>
-      <c r="F37" s="106" t="s">
-        <v>130</v>
-      </c>
-      <c r="G37" s="107"/>
-      <c r="H37" s="106" t="s">
-        <v>93</v>
-      </c>
-      <c r="I37" s="107"/>
-      <c r="J37" s="109" t="s">
-        <v>98</v>
-      </c>
-      <c r="K37" s="110"/>
+      <c r="B37" s="174" t="s">
+        <v>126</v>
+      </c>
+      <c r="C37" s="174"/>
+      <c r="D37" s="174" t="s">
+        <v>96</v>
+      </c>
+      <c r="E37" s="174"/>
+      <c r="F37" s="175" t="s">
+        <v>127</v>
+      </c>
+      <c r="G37" s="176"/>
+      <c r="H37" s="175" t="s">
+        <v>90</v>
+      </c>
+      <c r="I37" s="176"/>
+      <c r="J37" s="178" t="s">
+        <v>95</v>
+      </c>
+      <c r="K37" s="179"/>
       <c r="L37" s="43"/>
       <c r="M37" s="69"/>
       <c r="N37" s="70"/>
@@ -7865,39 +7868,39 @@
         <v>11</v>
       </c>
       <c r="Q37" s="68" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="R37" s="68" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="38" spans="1:22" ht="27" customHeight="1">
       <c r="A38" s="43"/>
-      <c r="B38" s="92">
+      <c r="B38" s="180">
         <v>0</v>
       </c>
-      <c r="C38" s="93"/>
-      <c r="D38" s="96">
+      <c r="C38" s="181"/>
+      <c r="D38" s="184">
         <v>0</v>
       </c>
-      <c r="E38" s="97"/>
-      <c r="F38" s="92">
+      <c r="E38" s="185"/>
+      <c r="F38" s="180">
         <v>0</v>
       </c>
-      <c r="G38" s="93"/>
-      <c r="H38" s="92">
+      <c r="G38" s="181"/>
+      <c r="H38" s="180">
         <v>0</v>
       </c>
-      <c r="I38" s="93"/>
-      <c r="J38" s="101">
+      <c r="I38" s="181"/>
+      <c r="J38" s="188">
         <v>0</v>
       </c>
-      <c r="K38" s="102"/>
+      <c r="K38" s="189"/>
       <c r="L38" s="71"/>
-      <c r="M38" s="100" t="s">
-        <v>131</v>
-      </c>
-      <c r="N38" s="100"/>
+      <c r="M38" s="133" t="s">
+        <v>128</v>
+      </c>
+      <c r="N38" s="133"/>
       <c r="O38" s="86">
         <v>0</v>
       </c>
@@ -7913,21 +7916,21 @@
     </row>
     <row r="39" spans="1:22" ht="27" customHeight="1">
       <c r="A39" s="43"/>
-      <c r="B39" s="94"/>
-      <c r="C39" s="95"/>
-      <c r="D39" s="98"/>
-      <c r="E39" s="99"/>
-      <c r="F39" s="94"/>
-      <c r="G39" s="95"/>
-      <c r="H39" s="94"/>
-      <c r="I39" s="95"/>
-      <c r="J39" s="103"/>
-      <c r="K39" s="104"/>
+      <c r="B39" s="182"/>
+      <c r="C39" s="183"/>
+      <c r="D39" s="186"/>
+      <c r="E39" s="187"/>
+      <c r="F39" s="182"/>
+      <c r="G39" s="183"/>
+      <c r="H39" s="182"/>
+      <c r="I39" s="183"/>
+      <c r="J39" s="190"/>
+      <c r="K39" s="191"/>
       <c r="L39" s="71"/>
-      <c r="M39" s="100" t="s">
-        <v>132</v>
-      </c>
-      <c r="N39" s="100"/>
+      <c r="M39" s="133" t="s">
+        <v>129</v>
+      </c>
+      <c r="N39" s="133"/>
       <c r="O39" s="86">
         <v>0</v>
       </c>
@@ -8207,6 +8210,79 @@
     </row>
   </sheetData>
   <mergeCells count="89">
+    <mergeCell ref="B38:C39"/>
+    <mergeCell ref="D38:E39"/>
+    <mergeCell ref="F38:G39"/>
+    <mergeCell ref="H38:I39"/>
+    <mergeCell ref="M39:N39"/>
+    <mergeCell ref="M38:N38"/>
+    <mergeCell ref="J38:K39"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="B36:R36"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="B29:R29"/>
+    <mergeCell ref="B32:R32"/>
+    <mergeCell ref="P33:R34"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="I34:K34"/>
+    <mergeCell ref="L34:M34"/>
+    <mergeCell ref="N34:O34"/>
+    <mergeCell ref="B31:R31"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="I33:K33"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="N33:O33"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="L27:R27"/>
+    <mergeCell ref="K21:M25"/>
+    <mergeCell ref="N21:O25"/>
+    <mergeCell ref="P21:R25"/>
+    <mergeCell ref="K19:R19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="E20:I20"/>
+    <mergeCell ref="P20:R20"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:R1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:R3"/>
+    <mergeCell ref="B4:R4"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="N5:P5"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="K7:R7"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:I8"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="D15:E16"/>
+    <mergeCell ref="B15:C16"/>
+    <mergeCell ref="H15:I16"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:I9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:I10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:I11"/>
+    <mergeCell ref="B14:R14"/>
+    <mergeCell ref="B17:C17"/>
     <mergeCell ref="M15:N16"/>
     <mergeCell ref="O15:P16"/>
     <mergeCell ref="Q15:R16"/>
@@ -8223,79 +8299,6 @@
     <mergeCell ref="H21:I21"/>
     <mergeCell ref="Q17:R17"/>
     <mergeCell ref="B19:I19"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:I8"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="D15:E16"/>
-    <mergeCell ref="B15:C16"/>
-    <mergeCell ref="H15:I16"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:I9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:I10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:I11"/>
-    <mergeCell ref="B14:R14"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="N5:P5"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="K7:R7"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:R1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:R3"/>
-    <mergeCell ref="B4:R4"/>
-    <mergeCell ref="K19:R19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="E20:I20"/>
-    <mergeCell ref="P20:R20"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="N20:O20"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="L27:R27"/>
-    <mergeCell ref="K21:M25"/>
-    <mergeCell ref="N21:O25"/>
-    <mergeCell ref="P21:R25"/>
-    <mergeCell ref="B29:R29"/>
-    <mergeCell ref="B32:R32"/>
-    <mergeCell ref="P33:R34"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="I34:K34"/>
-    <mergeCell ref="L34:M34"/>
-    <mergeCell ref="N34:O34"/>
-    <mergeCell ref="B31:R31"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="I33:K33"/>
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="N33:O33"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="B36:R36"/>
-    <mergeCell ref="J37:K37"/>
-    <mergeCell ref="B38:C39"/>
-    <mergeCell ref="D38:E39"/>
-    <mergeCell ref="F38:G39"/>
-    <mergeCell ref="H38:I39"/>
-    <mergeCell ref="M39:N39"/>
-    <mergeCell ref="M38:N38"/>
-    <mergeCell ref="J38:K39"/>
   </mergeCells>
   <conditionalFormatting sqref="K28:O28 L27">
     <cfRule type="dataBar" priority="2">
@@ -8406,7 +8409,7 @@
     <row r="2" spans="1:8" ht="18">
       <c r="A2" s="1"/>
       <c r="B2" s="192" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C2" s="192"/>
       <c r="D2" s="192"/>
@@ -8428,11 +8431,11 @@
     <row r="4" spans="1:8" ht="30" customHeight="1">
       <c r="A4" s="1"/>
       <c r="B4" s="199" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C4" s="200"/>
       <c r="D4" s="197" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E4" s="197"/>
       <c r="F4" s="197"/>
@@ -8444,7 +8447,7 @@
       <c r="B5" s="201"/>
       <c r="C5" s="202"/>
       <c r="D5" s="198" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E5" s="198"/>
       <c r="F5" s="198"/>
@@ -8464,11 +8467,11 @@
     <row r="7" spans="1:8" ht="39.75" customHeight="1">
       <c r="A7" s="1"/>
       <c r="B7" s="203" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C7" s="203"/>
       <c r="D7" s="196" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E7" s="194"/>
       <c r="F7" s="194"/>
@@ -8480,7 +8483,7 @@
       <c r="B8" s="203"/>
       <c r="C8" s="203"/>
       <c r="D8" s="193" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E8" s="194"/>
       <c r="F8" s="194"/>
@@ -8500,13 +8503,13 @@
     <row r="10" spans="1:8" ht="24">
       <c r="A10" s="1"/>
       <c r="B10" s="32" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>9</v>
@@ -8515,7 +8518,7 @@
         <v>8</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H10" s="9" t="s">
         <v>10</v>
@@ -11413,10 +11416,10 @@
     <row r="4" spans="1:16" s="74" customFormat="1" ht="52.5" customHeight="1">
       <c r="A4" s="72"/>
       <c r="B4" s="75" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C4" s="205" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D4" s="205"/>
       <c r="E4" s="205"/>
@@ -11453,7 +11456,7 @@
     <row r="6" spans="1:16">
       <c r="A6" s="2"/>
       <c r="B6" s="33" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C6" s="34" t="s">
         <v>5</v>
@@ -12434,10 +12437,10 @@
     <row r="4" spans="1:16" s="74" customFormat="1" ht="39.75" customHeight="1">
       <c r="A4" s="72"/>
       <c r="B4" s="75" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C4" s="205" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D4" s="205"/>
       <c r="E4" s="205"/>
@@ -12474,7 +12477,7 @@
     <row r="6" spans="1:16">
       <c r="A6" s="2"/>
       <c r="B6" s="33" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C6" s="34" t="s">
         <v>1</v>
@@ -13900,7 +13903,7 @@
     <row r="2" spans="1:14" customFormat="1" ht="18">
       <c r="A2" s="1"/>
       <c r="B2" s="204" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C2" s="204"/>
       <c r="D2" s="204"/>
@@ -13916,48 +13919,48 @@
       <c r="N2" s="1"/>
     </row>
     <row r="4" spans="1:14" ht="77.25" customHeight="1">
-      <c r="B4" s="212" t="s">
-        <v>123</v>
-      </c>
-      <c r="C4" s="213"/>
-      <c r="D4" s="214" t="s">
-        <v>117</v>
-      </c>
-      <c r="E4" s="215"/>
-      <c r="F4" s="215"/>
-      <c r="G4" s="215"/>
-      <c r="H4" s="216"/>
+      <c r="B4" s="209" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" s="210"/>
+      <c r="D4" s="211" t="s">
+        <v>114</v>
+      </c>
+      <c r="E4" s="212"/>
+      <c r="F4" s="212"/>
+      <c r="G4" s="212"/>
+      <c r="H4" s="213"/>
     </row>
     <row r="6" spans="1:14" ht="21" customHeight="1">
-      <c r="B6" s="207" t="s">
-        <v>102</v>
-      </c>
-      <c r="C6" s="207"/>
-      <c r="D6" s="207"/>
-      <c r="E6" s="207"/>
-      <c r="F6" s="207"/>
-      <c r="G6" s="207"/>
-      <c r="H6" s="207"/>
+      <c r="B6" s="214" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" s="214"/>
+      <c r="D6" s="214"/>
+      <c r="E6" s="214"/>
+      <c r="F6" s="214"/>
+      <c r="G6" s="214"/>
+      <c r="H6" s="214"/>
     </row>
     <row r="7" spans="1:14" ht="23.25" customHeight="1">
-      <c r="B7" s="210" t="s">
-        <v>100</v>
-      </c>
-      <c r="C7" s="211"/>
+      <c r="B7" s="207" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" s="208"/>
       <c r="D7" s="84" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="84" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" s="84" t="s">
         <v>53</v>
       </c>
-      <c r="E7" s="84" t="s">
+      <c r="G7" s="84" t="s">
         <v>54</v>
       </c>
-      <c r="F7" s="84" t="s">
+      <c r="H7" s="84" t="s">
         <v>55</v>
-      </c>
-      <c r="G7" s="84" t="s">
-        <v>56</v>
-      </c>
-      <c r="H7" s="84" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:14" s="85" customFormat="1" ht="27" customHeight="1">
@@ -13973,7 +13976,7 @@
     </row>
     <row r="9" spans="1:14" s="85" customFormat="1" ht="27" customHeight="1">
       <c r="B9" s="206" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C9" s="206"/>
       <c r="D9" s="91"/>
@@ -13984,7 +13987,7 @@
     </row>
     <row r="10" spans="1:14" s="85" customFormat="1" ht="27" customHeight="1">
       <c r="B10" s="206" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C10" s="206"/>
       <c r="D10" s="91"/>
@@ -13995,7 +13998,7 @@
     </row>
     <row r="11" spans="1:14" s="85" customFormat="1" ht="27" customHeight="1">
       <c r="B11" s="206" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C11" s="206"/>
       <c r="D11" s="91"/>
@@ -14006,7 +14009,7 @@
     </row>
     <row r="12" spans="1:14" s="85" customFormat="1" ht="27" customHeight="1">
       <c r="B12" s="206" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C12" s="206"/>
       <c r="D12" s="91"/>
@@ -14017,7 +14020,7 @@
     </row>
     <row r="13" spans="1:14" s="85" customFormat="1" ht="27" customHeight="1">
       <c r="B13" s="206" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C13" s="206"/>
       <c r="D13" s="91"/>
@@ -14028,7 +14031,7 @@
     </row>
     <row r="14" spans="1:14" s="85" customFormat="1" ht="27" customHeight="1">
       <c r="B14" s="206" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C14" s="206"/>
       <c r="D14" s="91"/>
@@ -14043,106 +14046,106 @@
       <c r="D15"/>
     </row>
     <row r="16" spans="1:14" ht="20.25" customHeight="1">
-      <c r="B16" s="207" t="s">
-        <v>127</v>
-      </c>
-      <c r="C16" s="207"/>
-      <c r="D16" s="207"/>
-      <c r="E16" s="207"/>
-      <c r="F16" s="207"/>
-      <c r="G16" s="207"/>
-      <c r="H16" s="207"/>
+      <c r="B16" s="214" t="s">
+        <v>124</v>
+      </c>
+      <c r="C16" s="214"/>
+      <c r="D16" s="214"/>
+      <c r="E16" s="214"/>
+      <c r="F16" s="214"/>
+      <c r="G16" s="214"/>
+      <c r="H16" s="214"/>
     </row>
     <row r="17" spans="2:8" ht="37.5" customHeight="1">
-      <c r="B17" s="208" t="s">
+      <c r="B17" s="215" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="215"/>
+      <c r="D17" s="216" t="s">
+        <v>122</v>
+      </c>
+      <c r="E17" s="216"/>
+      <c r="F17" s="216"/>
+      <c r="G17" s="216"/>
+      <c r="H17" s="216"/>
+    </row>
+    <row r="18" spans="2:8" ht="37.5" customHeight="1">
+      <c r="B18" s="215" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" s="215"/>
+      <c r="D18" s="216" t="s">
+        <v>123</v>
+      </c>
+      <c r="E18" s="216"/>
+      <c r="F18" s="216"/>
+      <c r="G18" s="216"/>
+      <c r="H18" s="216"/>
+    </row>
+    <row r="19" spans="2:8" ht="37.5" customHeight="1">
+      <c r="B19" s="215" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" s="215"/>
+      <c r="D19" s="216" t="s">
+        <v>82</v>
+      </c>
+      <c r="E19" s="216"/>
+      <c r="F19" s="216"/>
+      <c r="G19" s="216"/>
+      <c r="H19" s="216"/>
+    </row>
+    <row r="20" spans="2:8" ht="37.5" customHeight="1">
+      <c r="B20" s="215" t="s">
         <v>78</v>
       </c>
-      <c r="C17" s="208"/>
-      <c r="D17" s="209" t="s">
-        <v>125</v>
-      </c>
-      <c r="E17" s="209"/>
-      <c r="F17" s="209"/>
-      <c r="G17" s="209"/>
-      <c r="H17" s="209"/>
-    </row>
-    <row r="18" spans="2:8" ht="37.5" customHeight="1">
-      <c r="B18" s="208" t="s">
+      <c r="C20" s="215"/>
+      <c r="D20" s="216" t="s">
+        <v>83</v>
+      </c>
+      <c r="E20" s="216"/>
+      <c r="F20" s="216"/>
+      <c r="G20" s="216"/>
+      <c r="H20" s="216"/>
+    </row>
+    <row r="21" spans="2:8" ht="37.5" customHeight="1">
+      <c r="B21" s="215" t="s">
         <v>79</v>
       </c>
-      <c r="C18" s="208"/>
-      <c r="D18" s="209" t="s">
-        <v>126</v>
-      </c>
-      <c r="E18" s="209"/>
-      <c r="F18" s="209"/>
-      <c r="G18" s="209"/>
-      <c r="H18" s="209"/>
-    </row>
-    <row r="19" spans="2:8" ht="37.5" customHeight="1">
-      <c r="B19" s="208" t="s">
+      <c r="C21" s="215"/>
+      <c r="D21" s="216" t="s">
+        <v>84</v>
+      </c>
+      <c r="E21" s="216"/>
+      <c r="F21" s="216"/>
+      <c r="G21" s="216"/>
+      <c r="H21" s="216"/>
+    </row>
+    <row r="22" spans="2:8" ht="37.5" customHeight="1">
+      <c r="B22" s="215" t="s">
         <v>80</v>
       </c>
-      <c r="C19" s="208"/>
-      <c r="D19" s="209" t="s">
+      <c r="C22" s="215"/>
+      <c r="D22" s="216" t="s">
         <v>85</v>
       </c>
-      <c r="E19" s="209"/>
-      <c r="F19" s="209"/>
-      <c r="G19" s="209"/>
-      <c r="H19" s="209"/>
-    </row>
-    <row r="20" spans="2:8" ht="37.5" customHeight="1">
-      <c r="B20" s="208" t="s">
+      <c r="E22" s="216"/>
+      <c r="F22" s="216"/>
+      <c r="G22" s="216"/>
+      <c r="H22" s="216"/>
+    </row>
+    <row r="23" spans="2:8" ht="37.5" customHeight="1">
+      <c r="B23" s="215" t="s">
         <v>81</v>
       </c>
-      <c r="C20" s="208"/>
-      <c r="D20" s="209" t="s">
+      <c r="C23" s="215"/>
+      <c r="D23" s="216" t="s">
         <v>86</v>
       </c>
-      <c r="E20" s="209"/>
-      <c r="F20" s="209"/>
-      <c r="G20" s="209"/>
-      <c r="H20" s="209"/>
-    </row>
-    <row r="21" spans="2:8" ht="37.5" customHeight="1">
-      <c r="B21" s="208" t="s">
-        <v>82</v>
-      </c>
-      <c r="C21" s="208"/>
-      <c r="D21" s="209" t="s">
-        <v>87</v>
-      </c>
-      <c r="E21" s="209"/>
-      <c r="F21" s="209"/>
-      <c r="G21" s="209"/>
-      <c r="H21" s="209"/>
-    </row>
-    <row r="22" spans="2:8" ht="37.5" customHeight="1">
-      <c r="B22" s="208" t="s">
-        <v>83</v>
-      </c>
-      <c r="C22" s="208"/>
-      <c r="D22" s="209" t="s">
-        <v>88</v>
-      </c>
-      <c r="E22" s="209"/>
-      <c r="F22" s="209"/>
-      <c r="G22" s="209"/>
-      <c r="H22" s="209"/>
-    </row>
-    <row r="23" spans="2:8" ht="37.5" customHeight="1">
-      <c r="B23" s="208" t="s">
-        <v>84</v>
-      </c>
-      <c r="C23" s="208"/>
-      <c r="D23" s="209" t="s">
-        <v>89</v>
-      </c>
-      <c r="E23" s="209"/>
-      <c r="F23" s="209"/>
-      <c r="G23" s="209"/>
-      <c r="H23" s="209"/>
+      <c r="E23" s="216"/>
+      <c r="F23" s="216"/>
+      <c r="G23" s="216"/>
+      <c r="H23" s="216"/>
     </row>
     <row r="24" spans="2:8" ht="15">
       <c r="B24"/>
@@ -14414,17 +14417,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:H4"/>
-    <mergeCell ref="B6:H6"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B16:H16"/>
     <mergeCell ref="B23:C23"/>
@@ -14441,6 +14433,17 @@
     <mergeCell ref="D21:H21"/>
     <mergeCell ref="D20:H20"/>
     <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:H4"/>
+    <mergeCell ref="B6:H6"/>
   </mergeCells>
   <conditionalFormatting sqref="D8:H14">
     <cfRule type="dataBar" priority="1">
@@ -14522,7 +14525,7 @@
     <row r="2" spans="1:16" ht="18">
       <c r="A2" s="1"/>
       <c r="B2" s="204" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C2" s="204"/>
       <c r="D2" s="204"/>
@@ -14560,10 +14563,10 @@
     <row r="4" spans="1:16">
       <c r="A4" s="2"/>
       <c r="B4" s="218" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C4" s="220" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D4" s="221"/>
       <c r="E4" s="221"/>
@@ -14618,7 +14621,7 @@
     <row r="7" spans="1:16" ht="15" customHeight="1">
       <c r="A7" s="2"/>
       <c r="B7" s="226" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C7" s="226"/>
       <c r="D7" s="226"/>
@@ -14656,7 +14659,7 @@
     <row r="9" spans="1:16">
       <c r="A9" s="2"/>
       <c r="B9" s="217" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C9" s="217"/>
       <c r="D9" s="217"/>
@@ -15071,7 +15074,7 @@
     <row r="32" spans="1:16">
       <c r="A32" s="2"/>
       <c r="B32" s="217" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C32" s="217"/>
       <c r="D32" s="217"/>
@@ -15683,7 +15686,7 @@
     <row r="2" spans="1:12" ht="18" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="204" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C2" s="204"/>
       <c r="D2" s="204"/>
@@ -15713,14 +15716,14 @@
     <row r="4" spans="1:12" ht="15" customHeight="1">
       <c r="A4" s="2"/>
       <c r="B4" s="228" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C4" s="228"/>
-      <c r="D4" s="214" t="s">
-        <v>90</v>
-      </c>
-      <c r="E4" s="215"/>
-      <c r="F4" s="216"/>
+      <c r="D4" s="211" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" s="212"/>
+      <c r="F4" s="213"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -15745,7 +15748,7 @@
     <row r="6" spans="1:12" ht="16.5">
       <c r="A6" s="2"/>
       <c r="B6" s="227" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C6" s="227"/>
       <c r="D6" s="227"/>
@@ -15761,19 +15764,19 @@
     <row r="7" spans="1:12">
       <c r="A7" s="2"/>
       <c r="B7" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="D7" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>66</v>
-      </c>
       <c r="F7" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -19594,7 +19597,7 @@
     <row r="2" spans="1:16" ht="18">
       <c r="A2" s="1"/>
       <c r="B2" s="204" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C2" s="204"/>
       <c r="D2" s="204"/>
@@ -19632,10 +19635,10 @@
     <row r="4" spans="1:16" ht="40.5" customHeight="1">
       <c r="A4" s="2"/>
       <c r="B4" s="82" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C4" s="229" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D4" s="229"/>
       <c r="E4" s="229"/>
@@ -19671,7 +19674,7 @@
     </row>
     <row r="6" spans="1:16" ht="16.5">
       <c r="B6" s="14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C6" s="14">
         <v>2014</v>
@@ -19694,7 +19697,7 @@
     </row>
     <row r="7" spans="1:16">
       <c r="B7" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C7" s="29"/>
       <c r="D7" s="29"/>
@@ -19705,7 +19708,7 @@
     </row>
     <row r="8" spans="1:16">
       <c r="B8" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C8" s="27"/>
       <c r="D8" s="27"/>
@@ -19716,7 +19719,7 @@
     </row>
     <row r="9" spans="1:16">
       <c r="B9" s="13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C9" s="29"/>
       <c r="D9" s="29"/>
@@ -19736,7 +19739,7 @@
     </row>
     <row r="11" spans="1:16">
       <c r="B11" s="12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C11" s="28">
         <f>SUM(C7:C9)</f>
@@ -19803,7 +19806,7 @@
     <row r="1" spans="1:9" ht="15">
       <c r="A1" s="11"/>
       <c r="B1" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
@@ -19811,12 +19814,12 @@
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
       <c r="H1" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B2" s="11" t="e">
         <f>IF(C2=0,NA(),C2)</f>
@@ -19829,7 +19832,7 @@
       <c r="E2" s="11"/>
       <c r="F2" s="11"/>
       <c r="G2" s="11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H2" s="11" t="e">
         <f>IF(I2=0,NA(),I2)</f>
@@ -19841,7 +19844,7 @@
     </row>
     <row r="3" spans="1:9" ht="15">
       <c r="A3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B3" s="11" t="e">
         <f t="shared" ref="B3:B6" si="0">IF(C3=0,NA(),C3)</f>
@@ -19854,7 +19857,7 @@
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
       <c r="G3" s="11" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H3" s="11" t="e">
         <f t="shared" ref="H3:H6" si="1">IF(I3=0,NA(),I3)</f>
@@ -19866,7 +19869,7 @@
     </row>
     <row r="4" spans="1:9" ht="15">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B4" s="11" t="e">
         <f t="shared" si="0"/>
@@ -19879,7 +19882,7 @@
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
       <c r="G4" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H4" s="11" t="e">
         <f t="shared" si="1"/>
@@ -19891,7 +19894,7 @@
     </row>
     <row r="5" spans="1:9" ht="15">
       <c r="A5" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B5" s="11" t="e">
         <f t="shared" si="0"/>
@@ -19904,7 +19907,7 @@
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
       <c r="G5" s="11" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="H5" s="11" t="e">
         <f t="shared" si="1"/>
@@ -19916,7 +19919,7 @@
     </row>
     <row r="6" spans="1:9" ht="15">
       <c r="A6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B6" s="11" t="e">
         <f t="shared" si="0"/>
@@ -19929,7 +19932,7 @@
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
       <c r="G6" s="11" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="H6" s="11" t="e">
         <f t="shared" si="1"/>
@@ -19941,7 +19944,7 @@
     </row>
     <row r="7" spans="1:9" ht="15">
       <c r="A7" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B7" s="11">
         <f>IF(AND(ISNA(B6),ISNA(B5),ISNA(B4),ISNA(B3),ISNA(B2)),0,NA())</f>
@@ -19949,7 +19952,7 @@
       </c>
       <c r="C7" s="11"/>
       <c r="G7" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H7" s="11">
         <f>IF(AND(ISNA(H6),ISNA(H5),ISNA(H4),ISNA(H3),ISNA(H2)),0,NA())</f>
@@ -19959,7 +19962,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="B8" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:9">

</xml_diff>